<commit_message>
change construciton properties to avoid merging conflicts
</commit_message>
<xml_diff>
--- a/cea/databases/SIN/archetypes/construction_properties.xlsx
+++ b/cea/databases/SIN/archetypes/construction_properties.xlsx
@@ -5,11 +5,11 @@
   <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Jimeno\Documents\CityEnergyAnalyst\cea\databases\archetypes\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Jimeno\Documents\CityEnergyAnalyst\cea\databases\SIN\archetypes\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="458" windowWidth="38400" windowHeight="22020" tabRatio="785" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="458" windowWidth="38400" windowHeight="22020" tabRatio="785" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="ARCHITECTURE" sheetId="3" r:id="rId1"/>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="420" uniqueCount="68">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="441" uniqueCount="69">
   <si>
     <t>Code</t>
   </si>
@@ -234,6 +234,9 @@
   </si>
   <si>
     <t>T4</t>
+  </si>
+  <si>
+    <t>UNIVERSITY</t>
   </si>
 </sst>
 </file>
@@ -1117,13 +1120,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:Q19"/>
+  <dimension ref="A1:Q20"/>
   <sheetViews>
     <sheetView zoomScale="85" zoomScaleNormal="85" zoomScalePageLayoutView="85" workbookViewId="0">
       <pane xSplit="4" ySplit="1" topLeftCell="E2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="D1" sqref="D1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="I24" sqref="I24"/>
+      <selection pane="bottomRight" activeCell="H10" sqref="H10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.1328125" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -1566,7 +1569,7 @@
     </row>
     <row r="10" spans="1:17" x14ac:dyDescent="0.45">
       <c r="A10" s="6" t="s">
-        <v>24</v>
+        <v>68</v>
       </c>
       <c r="B10" s="6" t="s">
         <v>60</v>
@@ -1599,7 +1602,7 @@
         <v>50</v>
       </c>
       <c r="L10" s="3" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
       <c r="M10" s="3" t="s">
         <v>52</v>
@@ -1613,7 +1616,7 @@
     </row>
     <row r="11" spans="1:17" x14ac:dyDescent="0.45">
       <c r="A11" s="6" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B11" s="6" t="s">
         <v>60</v>
@@ -1625,7 +1628,7 @@
         <v>47</v>
       </c>
       <c r="E11" s="3">
-        <v>0.84</v>
+        <v>0.67</v>
       </c>
       <c r="F11" s="3">
         <v>0.35</v>
@@ -1646,7 +1649,7 @@
         <v>50</v>
       </c>
       <c r="L11" s="3" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="M11" s="3" t="s">
         <v>52</v>
@@ -1660,7 +1663,7 @@
     </row>
     <row r="12" spans="1:17" x14ac:dyDescent="0.45">
       <c r="A12" s="6" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B12" s="6" t="s">
         <v>60</v>
@@ -1672,7 +1675,7 @@
         <v>47</v>
       </c>
       <c r="E12" s="3">
-        <v>0.67</v>
+        <v>0.84</v>
       </c>
       <c r="F12" s="3">
         <v>0.35</v>
@@ -1693,7 +1696,7 @@
         <v>50</v>
       </c>
       <c r="L12" s="3" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
       <c r="M12" s="3" t="s">
         <v>52</v>
@@ -1707,7 +1710,7 @@
     </row>
     <row r="13" spans="1:17" x14ac:dyDescent="0.45">
       <c r="A13" s="6" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="B13" s="6" t="s">
         <v>60</v>
@@ -1719,7 +1722,7 @@
         <v>47</v>
       </c>
       <c r="E13" s="3">
-        <v>0</v>
+        <v>0.67</v>
       </c>
       <c r="F13" s="3">
         <v>0.35</v>
@@ -1740,21 +1743,21 @@
         <v>50</v>
       </c>
       <c r="L13" s="3" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="M13" s="3" t="s">
         <v>52</v>
       </c>
       <c r="N13" s="3" t="s">
-        <v>51</v>
+        <v>53</v>
       </c>
       <c r="O13" s="3" t="s">
-        <v>54</v>
+        <v>50</v>
       </c>
     </row>
     <row r="14" spans="1:17" x14ac:dyDescent="0.45">
       <c r="A14" s="6" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="B14" s="6" t="s">
         <v>60</v>
@@ -1766,19 +1769,19 @@
         <v>47</v>
       </c>
       <c r="E14" s="3">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F14" s="3">
-        <v>0</v>
+        <v>0.35</v>
       </c>
       <c r="G14" s="3">
-        <v>0</v>
+        <v>0.35</v>
       </c>
       <c r="H14" s="3">
-        <v>0</v>
+        <v>0.35</v>
       </c>
       <c r="I14" s="3">
-        <v>0</v>
+        <v>0.35</v>
       </c>
       <c r="J14" s="3" t="s">
         <v>51</v>
@@ -1793,15 +1796,15 @@
         <v>52</v>
       </c>
       <c r="N14" s="3" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="O14" s="3" t="s">
-        <v>50</v>
+        <v>54</v>
       </c>
     </row>
     <row r="15" spans="1:17" x14ac:dyDescent="0.45">
       <c r="A15" s="6" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="B15" s="6" t="s">
         <v>60</v>
@@ -1813,42 +1816,42 @@
         <v>47</v>
       </c>
       <c r="E15" s="3">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F15" s="3">
-        <v>0.5</v>
+        <v>0</v>
       </c>
       <c r="G15" s="3">
-        <v>0.5</v>
+        <v>0</v>
       </c>
       <c r="H15" s="3">
-        <v>0.5</v>
+        <v>0</v>
       </c>
       <c r="I15" s="3">
-        <v>0.5</v>
+        <v>0</v>
       </c>
       <c r="J15" s="3" t="s">
         <v>51</v>
       </c>
       <c r="K15" s="3" t="s">
-        <v>53</v>
+        <v>50</v>
       </c>
       <c r="L15" s="3" t="s">
-        <v>50</v>
+        <v>58</v>
       </c>
       <c r="M15" s="3" t="s">
         <v>52</v>
       </c>
       <c r="N15" s="3" t="s">
-        <v>51</v>
+        <v>53</v>
       </c>
       <c r="O15" s="3" t="s">
-        <v>54</v>
+        <v>50</v>
       </c>
     </row>
     <row r="16" spans="1:17" x14ac:dyDescent="0.45">
       <c r="A16" s="6" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B16" s="6" t="s">
         <v>60</v>
@@ -1860,25 +1863,25 @@
         <v>47</v>
       </c>
       <c r="E16" s="3">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F16" s="3">
-        <v>0</v>
+        <v>0.5</v>
       </c>
       <c r="G16" s="3">
-        <v>0</v>
+        <v>0.5</v>
       </c>
       <c r="H16" s="3">
-        <v>0</v>
+        <v>0.5</v>
       </c>
       <c r="I16" s="3">
-        <v>0</v>
+        <v>0.5</v>
       </c>
       <c r="J16" s="3" t="s">
         <v>51</v>
       </c>
       <c r="K16" s="3" t="s">
-        <v>50</v>
+        <v>53</v>
       </c>
       <c r="L16" s="3" t="s">
         <v>50</v>
@@ -1887,15 +1890,15 @@
         <v>52</v>
       </c>
       <c r="N16" s="3" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="O16" s="3" t="s">
-        <v>50</v>
+        <v>54</v>
       </c>
     </row>
     <row r="17" spans="1:15" x14ac:dyDescent="0.45">
       <c r="A17" s="6" t="s">
-        <v>40</v>
+        <v>30</v>
       </c>
       <c r="B17" s="6" t="s">
         <v>60</v>
@@ -1907,19 +1910,19 @@
         <v>47</v>
       </c>
       <c r="E17" s="3">
-        <v>0.67</v>
+        <v>1</v>
       </c>
       <c r="F17" s="3">
-        <v>0.35</v>
+        <v>0</v>
       </c>
       <c r="G17" s="3">
-        <v>0.35</v>
+        <v>0</v>
       </c>
       <c r="H17" s="3">
-        <v>0.35</v>
+        <v>0</v>
       </c>
       <c r="I17" s="3">
-        <v>0.35</v>
+        <v>0</v>
       </c>
       <c r="J17" s="3" t="s">
         <v>51</v>
@@ -1928,7 +1931,7 @@
         <v>50</v>
       </c>
       <c r="L17" s="3" t="s">
-        <v>57</v>
+        <v>50</v>
       </c>
       <c r="M17" s="3" t="s">
         <v>52</v>
@@ -1942,7 +1945,7 @@
     </row>
     <row r="18" spans="1:15" x14ac:dyDescent="0.45">
       <c r="A18" s="6" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="B18" s="6" t="s">
         <v>60</v>
@@ -1989,7 +1992,7 @@
     </row>
     <row r="19" spans="1:15" x14ac:dyDescent="0.45">
       <c r="A19" s="6" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="B19" s="6" t="s">
         <v>60</v>
@@ -2031,12 +2034,62 @@
         <v>53</v>
       </c>
       <c r="O19" s="3" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="20" spans="1:15" x14ac:dyDescent="0.45">
+      <c r="A20" s="6" t="s">
+        <v>42</v>
+      </c>
+      <c r="B20" s="6" t="s">
+        <v>60</v>
+      </c>
+      <c r="C20" s="6" t="s">
+        <v>59</v>
+      </c>
+      <c r="D20" s="2" t="s">
+        <v>47</v>
+      </c>
+      <c r="E20" s="3">
+        <v>0.67</v>
+      </c>
+      <c r="F20" s="3">
+        <v>0.35</v>
+      </c>
+      <c r="G20" s="3">
+        <v>0.35</v>
+      </c>
+      <c r="H20" s="3">
+        <v>0.35</v>
+      </c>
+      <c r="I20" s="3">
+        <v>0.35</v>
+      </c>
+      <c r="J20" s="3" t="s">
+        <v>51</v>
+      </c>
+      <c r="K20" s="3" t="s">
+        <v>50</v>
+      </c>
+      <c r="L20" s="3" t="s">
+        <v>57</v>
+      </c>
+      <c r="M20" s="3" t="s">
+        <v>52</v>
+      </c>
+      <c r="N20" s="3" t="s">
+        <v>53</v>
+      </c>
+      <c r="O20" s="3" t="s">
         <v>50</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+  <ignoredErrors>
+    <ignoredError sqref="B2:C20" numberStoredAsText="1"/>
+  </ignoredErrors>
 </worksheet>
 </file>
 
@@ -2044,11 +2097,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I1048576"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" zoomScalePageLayoutView="85" workbookViewId="0">
-      <pane xSplit="4" ySplit="1" topLeftCell="E2" activePane="bottomRight" state="frozen"/>
-      <selection pane="topRight" activeCell="D1" sqref="D1"/>
-      <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="K14" sqref="K14"/>
+    <sheetView zoomScale="85" zoomScaleNormal="85" zoomScalePageLayoutView="85" workbookViewId="0">
+      <selection activeCell="N17" sqref="N17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.1328125" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -2326,8 +2376,8 @@
       </c>
     </row>
     <row r="10" spans="1:9" x14ac:dyDescent="0.45">
-      <c r="A10" s="6" t="s">
-        <v>24</v>
+      <c r="A10" s="7" t="s">
+        <v>68</v>
       </c>
       <c r="B10" s="6" t="s">
         <v>60</v>
@@ -2356,7 +2406,7 @@
     </row>
     <row r="11" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A11" s="6" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B11" s="6" t="s">
         <v>60</v>
@@ -2374,7 +2424,7 @@
         <v>55</v>
       </c>
       <c r="G11" s="3" t="s">
-        <v>67</v>
+        <v>54</v>
       </c>
       <c r="H11" s="3" t="s">
         <v>51</v>
@@ -2385,7 +2435,7 @@
     </row>
     <row r="12" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A12" s="6" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B12" s="6" t="s">
         <v>60</v>
@@ -2414,7 +2464,7 @@
     </row>
     <row r="13" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A13" s="6" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="B13" s="6" t="s">
         <v>60</v>
@@ -2443,7 +2493,7 @@
     </row>
     <row r="14" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A14" s="6" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="B14" s="6" t="s">
         <v>60</v>
@@ -2461,7 +2511,7 @@
         <v>55</v>
       </c>
       <c r="G14" s="3" t="s">
-        <v>54</v>
+        <v>67</v>
       </c>
       <c r="H14" s="3" t="s">
         <v>51</v>
@@ -2472,7 +2522,7 @@
     </row>
     <row r="15" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A15" s="6" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="B15" s="6" t="s">
         <v>60</v>
@@ -2487,21 +2537,21 @@
         <v>54</v>
       </c>
       <c r="F15" s="3" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="G15" s="3" t="s">
         <v>54</v>
       </c>
       <c r="H15" s="3" t="s">
-        <v>54</v>
+        <v>51</v>
       </c>
       <c r="I15" s="3" t="s">
-        <v>54</v>
+        <v>50</v>
       </c>
     </row>
     <row r="16" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A16" s="6" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B16" s="6" t="s">
         <v>60</v>
@@ -2516,21 +2566,21 @@
         <v>54</v>
       </c>
       <c r="F16" s="3" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="G16" s="3" t="s">
         <v>54</v>
       </c>
       <c r="H16" s="3" t="s">
-        <v>51</v>
+        <v>54</v>
       </c>
       <c r="I16" s="3" t="s">
-        <v>50</v>
+        <v>54</v>
       </c>
     </row>
     <row r="17" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A17" s="6" t="s">
-        <v>40</v>
+        <v>30</v>
       </c>
       <c r="B17" s="6" t="s">
         <v>60</v>
@@ -2548,7 +2598,7 @@
         <v>55</v>
       </c>
       <c r="G17" s="3" t="s">
-        <v>67</v>
+        <v>54</v>
       </c>
       <c r="H17" s="3" t="s">
         <v>51</v>
@@ -2559,7 +2609,7 @@
     </row>
     <row r="18" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A18" s="6" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="B18" s="6" t="s">
         <v>60</v>
@@ -2577,7 +2627,7 @@
         <v>55</v>
       </c>
       <c r="G18" s="3" t="s">
-        <v>54</v>
+        <v>67</v>
       </c>
       <c r="H18" s="3" t="s">
         <v>51</v>
@@ -2588,7 +2638,7 @@
     </row>
     <row r="19" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A19" s="6" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="B19" s="6" t="s">
         <v>60</v>
@@ -2612,6 +2662,35 @@
         <v>51</v>
       </c>
       <c r="I19" s="3" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="20" spans="1:9" x14ac:dyDescent="0.45">
+      <c r="A20" s="6" t="s">
+        <v>42</v>
+      </c>
+      <c r="B20" s="6" t="s">
+        <v>60</v>
+      </c>
+      <c r="C20" s="6" t="s">
+        <v>59</v>
+      </c>
+      <c r="D20" s="2" t="s">
+        <v>47</v>
+      </c>
+      <c r="E20" s="3" t="s">
+        <v>54</v>
+      </c>
+      <c r="F20" s="3" t="s">
+        <v>55</v>
+      </c>
+      <c r="G20" s="3" t="s">
+        <v>54</v>
+      </c>
+      <c r="H20" s="3" t="s">
+        <v>51</v>
+      </c>
+      <c r="I20" s="3" t="s">
         <v>50</v>
       </c>
     </row>
@@ -2621,15 +2700,18 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+  <ignoredErrors>
+    <ignoredError sqref="B2:C9 B10:C20" numberStoredAsText="1"/>
+  </ignoredErrors>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F19"/>
+  <dimension ref="A1:F20"/>
   <sheetViews>
     <sheetView zoomScale="85" zoomScaleNormal="85" zoomScalePageLayoutView="85" workbookViewId="0">
-      <selection activeCell="H36" sqref="H36"/>
+      <selection activeCell="I14" sqref="I14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.1328125" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -2826,7 +2908,7 @@
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A10" s="6" t="s">
-        <v>24</v>
+        <v>68</v>
       </c>
       <c r="B10" s="8">
         <v>24</v>
@@ -2841,12 +2923,12 @@
         <v>10</v>
       </c>
       <c r="F10" s="8">
-        <v>8</v>
+        <v>10</v>
       </c>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A11" s="6" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B11" s="8">
         <v>24</v>
@@ -2854,19 +2936,19 @@
       <c r="C11" s="5">
         <v>10</v>
       </c>
-      <c r="D11" s="8">
-        <v>24</v>
+      <c r="D11" s="3">
+        <v>37</v>
       </c>
       <c r="E11" s="5">
         <v>10</v>
       </c>
       <c r="F11" s="8">
-        <v>10</v>
+        <v>8</v>
       </c>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A12" s="6" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B12" s="8">
         <v>24</v>
@@ -2874,8 +2956,8 @@
       <c r="C12" s="5">
         <v>10</v>
       </c>
-      <c r="D12" s="3">
-        <v>37</v>
+      <c r="D12" s="8">
+        <v>24</v>
       </c>
       <c r="E12" s="5">
         <v>10</v>
@@ -2886,36 +2968,36 @@
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A13" s="6" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="B13" s="8">
-        <v>50</v>
+        <v>24</v>
       </c>
       <c r="C13" s="5">
         <v>10</v>
       </c>
-      <c r="D13" s="5">
-        <v>50</v>
+      <c r="D13" s="3">
+        <v>37</v>
       </c>
       <c r="E13" s="5">
         <v>10</v>
       </c>
       <c r="F13" s="8">
-        <v>36</v>
+        <v>10</v>
       </c>
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A14" s="6" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="B14" s="8">
-        <v>24</v>
+        <v>50</v>
       </c>
       <c r="C14" s="5">
         <v>10</v>
       </c>
-      <c r="D14" s="8">
-        <v>24</v>
+      <c r="D14" s="5">
+        <v>50</v>
       </c>
       <c r="E14" s="5">
         <v>10</v>
@@ -2926,36 +3008,36 @@
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A15" s="6" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="B15" s="8">
-        <v>50</v>
+        <v>24</v>
       </c>
       <c r="C15" s="5">
         <v>10</v>
       </c>
-      <c r="D15" s="5">
-        <v>50</v>
+      <c r="D15" s="8">
+        <v>24</v>
       </c>
       <c r="E15" s="5">
         <v>10</v>
       </c>
       <c r="F15" s="8">
-        <v>0</v>
+        <v>36</v>
       </c>
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A16" s="6" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B16" s="8">
-        <v>-5</v>
+        <v>50</v>
       </c>
       <c r="C16" s="5">
         <v>10</v>
       </c>
-      <c r="D16" s="8">
-        <v>-5</v>
+      <c r="D16" s="5">
+        <v>50</v>
       </c>
       <c r="E16" s="5">
         <v>10</v>
@@ -2966,48 +3048,48 @@
     </row>
     <row r="17" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A17" s="6" t="s">
+        <v>30</v>
+      </c>
+      <c r="B17" s="8">
+        <v>-5</v>
+      </c>
+      <c r="C17" s="5">
+        <v>10</v>
+      </c>
+      <c r="D17" s="8">
+        <v>-5</v>
+      </c>
+      <c r="E17" s="5">
+        <v>10</v>
+      </c>
+      <c r="F17" s="8">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="18" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A18" s="6" t="s">
         <v>40</v>
       </c>
-      <c r="B17" s="8">
+      <c r="B18" s="8">
         <v>24</v>
       </c>
-      <c r="C17" s="5">
-        <v>10</v>
-      </c>
-      <c r="D17" s="3">
+      <c r="C18" s="5">
+        <v>10</v>
+      </c>
+      <c r="D18" s="3">
         <v>37</v>
       </c>
-      <c r="E17" s="5">
-        <v>10</v>
-      </c>
-      <c r="F17" s="8">
+      <c r="E18" s="5">
+        <v>10</v>
+      </c>
+      <c r="F18" s="8">
         <f>F9</f>
         <v>31</v>
       </c>
     </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.45">
-      <c r="A18" s="6" t="s">
-        <v>41</v>
-      </c>
-      <c r="B18" s="8">
-        <v>24</v>
-      </c>
-      <c r="C18" s="5">
-        <v>10</v>
-      </c>
-      <c r="D18" s="3">
-        <v>37</v>
-      </c>
-      <c r="E18" s="5">
-        <v>10</v>
-      </c>
-      <c r="F18" s="8">
-        <v>10</v>
-      </c>
-    </row>
     <row r="19" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A19" s="6" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="B19" s="8">
         <v>24</v>
@@ -3022,6 +3104,26 @@
         <v>10</v>
       </c>
       <c r="F19" s="8">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="20" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A20" s="6" t="s">
+        <v>42</v>
+      </c>
+      <c r="B20" s="8">
+        <v>24</v>
+      </c>
+      <c r="C20" s="5">
+        <v>10</v>
+      </c>
+      <c r="D20" s="3">
+        <v>37</v>
+      </c>
+      <c r="E20" s="5">
+        <v>10</v>
+      </c>
+      <c r="F20" s="8">
         <v>10</v>
       </c>
     </row>
@@ -3033,10 +3135,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:L22"/>
+  <dimension ref="A1:L23"/>
   <sheetViews>
-    <sheetView zoomScale="85" zoomScaleNormal="85" zoomScalePageLayoutView="85" workbookViewId="0">
-      <selection activeCell="P40" sqref="P40"/>
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" zoomScalePageLayoutView="85" workbookViewId="0">
+      <selection activeCell="Q19" sqref="Q19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.1328125" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -3398,7 +3500,7 @@
     </row>
     <row r="10" spans="1:12" x14ac:dyDescent="0.45">
       <c r="A10" s="6" t="s">
-        <v>24</v>
+        <v>68</v>
       </c>
       <c r="B10" s="8">
         <v>70</v>
@@ -3425,7 +3527,7 @@
         <v>0</v>
       </c>
       <c r="J10" s="8">
-        <v>4</v>
+        <v>20</v>
       </c>
       <c r="K10" s="5">
         <v>0</v>
@@ -3436,7 +3538,7 @@
     </row>
     <row r="11" spans="1:12" x14ac:dyDescent="0.45">
       <c r="A11" s="6" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B11" s="8">
         <v>70</v>
@@ -3445,10 +3547,10 @@
         <v>80</v>
       </c>
       <c r="D11" s="8">
-        <v>8</v>
+        <v>16</v>
       </c>
       <c r="E11" s="8">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="F11" s="8">
         <v>0</v>
@@ -3460,10 +3562,10 @@
         <v>0</v>
       </c>
       <c r="I11" s="8">
-        <v>40</v>
+        <v>0</v>
       </c>
       <c r="J11" s="8">
-        <v>80</v>
+        <v>4</v>
       </c>
       <c r="K11" s="5">
         <v>0</v>
@@ -3474,19 +3576,19 @@
     </row>
     <row r="12" spans="1:12" x14ac:dyDescent="0.45">
       <c r="A12" s="6" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B12" s="8">
-        <v>110</v>
+        <v>70</v>
       </c>
       <c r="C12" s="8">
-        <v>255</v>
+        <v>80</v>
       </c>
       <c r="D12" s="8">
-        <v>2</v>
+        <v>8</v>
       </c>
       <c r="E12" s="8">
-        <v>9.9</v>
+        <v>11</v>
       </c>
       <c r="F12" s="8">
         <v>0</v>
@@ -3498,7 +3600,7 @@
         <v>0</v>
       </c>
       <c r="I12" s="8">
-        <v>40</v>
+        <v>0</v>
       </c>
       <c r="J12" s="8">
         <v>80</v>
@@ -3512,19 +3614,19 @@
     </row>
     <row r="13" spans="1:12" x14ac:dyDescent="0.45">
       <c r="A13" s="6" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="B13" s="8">
-        <v>70</v>
+        <v>110</v>
       </c>
       <c r="C13" s="8">
-        <v>80</v>
+        <v>255</v>
       </c>
       <c r="D13" s="8">
         <v>2</v>
       </c>
       <c r="E13" s="8">
-        <v>11.3</v>
+        <v>9.9</v>
       </c>
       <c r="F13" s="8">
         <v>0</v>
@@ -3536,10 +3638,10 @@
         <v>0</v>
       </c>
       <c r="I13" s="8">
-        <v>0</v>
+        <v>40</v>
       </c>
       <c r="J13" s="8">
-        <v>360</v>
+        <v>80</v>
       </c>
       <c r="K13" s="5">
         <v>0</v>
@@ -3550,19 +3652,19 @@
     </row>
     <row r="14" spans="1:12" x14ac:dyDescent="0.45">
       <c r="A14" s="6" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="B14" s="8">
-        <v>0</v>
+        <v>70</v>
       </c>
       <c r="C14" s="8">
-        <v>0</v>
-      </c>
-      <c r="D14" s="9">
-        <v>0</v>
+        <v>80</v>
+      </c>
+      <c r="D14" s="8">
+        <v>2</v>
       </c>
       <c r="E14" s="8">
-        <v>7.1</v>
+        <v>11.3</v>
       </c>
       <c r="F14" s="8">
         <v>0</v>
@@ -3570,14 +3672,14 @@
       <c r="G14" s="8">
         <v>0</v>
       </c>
-      <c r="H14" s="8">
-        <v>500</v>
+      <c r="H14" s="5">
+        <v>0</v>
       </c>
       <c r="I14" s="8">
         <v>0</v>
       </c>
       <c r="J14" s="8">
-        <v>0</v>
+        <v>360</v>
       </c>
       <c r="K14" s="5">
         <v>0</v>
@@ -3588,7 +3690,7 @@
     </row>
     <row r="15" spans="1:12" x14ac:dyDescent="0.45">
       <c r="A15" s="6" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="B15" s="8">
         <v>0</v>
@@ -3596,11 +3698,11 @@
       <c r="C15" s="8">
         <v>0</v>
       </c>
-      <c r="D15" s="8">
+      <c r="D15" s="9">
         <v>0</v>
       </c>
       <c r="E15" s="8">
-        <v>5</v>
+        <v>7.1</v>
       </c>
       <c r="F15" s="8">
         <v>0</v>
@@ -3608,8 +3710,8 @@
       <c r="G15" s="8">
         <v>0</v>
       </c>
-      <c r="H15" s="5">
-        <v>0</v>
+      <c r="H15" s="8">
+        <v>500</v>
       </c>
       <c r="I15" s="8">
         <v>0</v>
@@ -3626,7 +3728,7 @@
     </row>
     <row r="16" spans="1:12" x14ac:dyDescent="0.45">
       <c r="A16" s="6" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B16" s="8">
         <v>0</v>
@@ -3638,13 +3740,13 @@
         <v>0</v>
       </c>
       <c r="E16" s="8">
-        <v>5.7</v>
+        <v>5</v>
       </c>
       <c r="F16" s="8">
         <v>0</v>
       </c>
       <c r="G16" s="8">
-        <v>5.6</v>
+        <v>0</v>
       </c>
       <c r="H16" s="5">
         <v>0</v>
@@ -3664,75 +3766,75 @@
     </row>
     <row r="17" spans="1:12" x14ac:dyDescent="0.45">
       <c r="A17" s="6" t="s">
+        <v>30</v>
+      </c>
+      <c r="B17" s="8">
+        <v>0</v>
+      </c>
+      <c r="C17" s="8">
+        <v>0</v>
+      </c>
+      <c r="D17" s="8">
+        <v>0</v>
+      </c>
+      <c r="E17" s="8">
+        <v>5.7</v>
+      </c>
+      <c r="F17" s="8">
+        <v>0</v>
+      </c>
+      <c r="G17" s="8">
+        <v>5.6</v>
+      </c>
+      <c r="H17" s="5">
+        <v>0</v>
+      </c>
+      <c r="I17" s="8">
+        <v>0</v>
+      </c>
+      <c r="J17" s="8">
+        <v>0</v>
+      </c>
+      <c r="K17" s="5">
+        <v>0</v>
+      </c>
+      <c r="L17" s="5">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="18" spans="1:12" x14ac:dyDescent="0.45">
+      <c r="A18" s="6" t="s">
         <v>40</v>
       </c>
-      <c r="B17" s="8">
-        <f>B11</f>
+      <c r="B18" s="8">
+        <f>B12</f>
         <v>70</v>
       </c>
-      <c r="C17" s="8">
-        <f>C11</f>
+      <c r="C18" s="8">
+        <f>C12</f>
         <v>80</v>
       </c>
-      <c r="D17" s="8">
+      <c r="D18" s="8">
         <v>30</v>
       </c>
-      <c r="E17" s="8">
+      <c r="E18" s="8">
         <v>12</v>
       </c>
-      <c r="F17" s="8">
+      <c r="F18" s="8">
         <f>F9</f>
         <v>16.5</v>
       </c>
-      <c r="G17" s="8">
-        <v>0</v>
-      </c>
-      <c r="H17" s="5">
-        <v>0</v>
-      </c>
-      <c r="I17" s="8">
-        <v>10</v>
-      </c>
-      <c r="J17" s="8">
+      <c r="G18" s="8">
+        <v>0</v>
+      </c>
+      <c r="H18" s="5">
+        <v>0</v>
+      </c>
+      <c r="I18" s="8">
+        <v>10</v>
+      </c>
+      <c r="J18" s="8">
         <v>20</v>
-      </c>
-      <c r="K17" s="5">
-        <v>0</v>
-      </c>
-      <c r="L17" s="5">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="18" spans="1:12" x14ac:dyDescent="0.45">
-      <c r="A18" s="6" t="s">
-        <v>41</v>
-      </c>
-      <c r="B18" s="8">
-        <v>70</v>
-      </c>
-      <c r="C18" s="8">
-        <v>80</v>
-      </c>
-      <c r="D18" s="8">
-        <v>7</v>
-      </c>
-      <c r="E18" s="8">
-        <v>10.8</v>
-      </c>
-      <c r="F18" s="8">
-        <v>0</v>
-      </c>
-      <c r="G18" s="8">
-        <v>0</v>
-      </c>
-      <c r="H18" s="5">
-        <v>0</v>
-      </c>
-      <c r="I18" s="8">
-        <v>0</v>
-      </c>
-      <c r="J18" s="8">
-        <v>4</v>
       </c>
       <c r="K18" s="5">
         <v>0</v>
@@ -3743,7 +3845,7 @@
     </row>
     <row r="19" spans="1:12" x14ac:dyDescent="0.45">
       <c r="A19" s="6" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="B19" s="8">
         <v>70</v>
@@ -3752,10 +3854,10 @@
         <v>80</v>
       </c>
       <c r="D19" s="8">
-        <v>2</v>
+        <v>7</v>
       </c>
       <c r="E19" s="8">
-        <v>6.9</v>
+        <v>10.8</v>
       </c>
       <c r="F19" s="8">
         <v>0</v>
@@ -3779,8 +3881,46 @@
         <v>0</v>
       </c>
     </row>
-    <row r="22" spans="1:12" x14ac:dyDescent="0.45">
-      <c r="G22" s="12"/>
+    <row r="20" spans="1:12" x14ac:dyDescent="0.45">
+      <c r="A20" s="6" t="s">
+        <v>42</v>
+      </c>
+      <c r="B20" s="8">
+        <v>70</v>
+      </c>
+      <c r="C20" s="8">
+        <v>80</v>
+      </c>
+      <c r="D20" s="8">
+        <v>2</v>
+      </c>
+      <c r="E20" s="8">
+        <v>6.9</v>
+      </c>
+      <c r="F20" s="8">
+        <v>0</v>
+      </c>
+      <c r="G20" s="8">
+        <v>0</v>
+      </c>
+      <c r="H20" s="5">
+        <v>0</v>
+      </c>
+      <c r="I20" s="8">
+        <v>0</v>
+      </c>
+      <c r="J20" s="8">
+        <v>4</v>
+      </c>
+      <c r="K20" s="5">
+        <v>0</v>
+      </c>
+      <c r="L20" s="5">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="23" spans="1:12" x14ac:dyDescent="0.45">
+      <c r="G23" s="12"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
fixing data helper and supply systems creator
</commit_message>
<xml_diff>
--- a/cea/databases/SIN/archetypes/construction_properties.xlsx
+++ b/cea/databases/SIN/archetypes/construction_properties.xlsx
@@ -9,15 +9,16 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="465" windowWidth="38400" windowHeight="22020" tabRatio="785"/>
+    <workbookView xWindow="0" yWindow="465" windowWidth="38400" windowHeight="22020" tabRatio="785" firstSheet="1" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="ARCHITECTURE" sheetId="3" r:id="rId1"/>
-    <sheet name="HVAC" sheetId="1" r:id="rId2"/>
-    <sheet name="INDOOR_COMFORT" sheetId="6" r:id="rId3"/>
-    <sheet name="INTERNAL_LOADS" sheetId="7" r:id="rId4"/>
+    <sheet name="SUPPLY" sheetId="8" r:id="rId2"/>
+    <sheet name="HVAC" sheetId="1" r:id="rId3"/>
+    <sheet name="INDOOR_COMFORT" sheetId="6" r:id="rId4"/>
+    <sheet name="INTERNAL_LOADS" sheetId="7" r:id="rId5"/>
   </sheets>
-  <calcPr calcId="162913" concurrentCalc="0"/>
+  <calcPr calcId="162913"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{79F54976-1DA5-4618-B147-4CDE4B953A38}">
       <x14:workbookPr defaultImageDpi="330"/>
@@ -30,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="442" uniqueCount="70">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="602" uniqueCount="71">
   <si>
     <t>Code</t>
   </si>
@@ -240,6 +241,9 @@
   </si>
   <si>
     <t>void_deck</t>
+  </si>
+  <si>
+    <t>type_el</t>
   </si>
 </sst>
 </file>
@@ -1125,7 +1129,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:R20"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" zoomScalePageLayoutView="85" workbookViewId="0">
+    <sheetView zoomScale="85" zoomScaleNormal="85" zoomScalePageLayoutView="85" workbookViewId="0">
       <pane xSplit="4" ySplit="1" topLeftCell="E2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="D1" sqref="D1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
@@ -2159,10 +2163,558 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:H1048576"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="H10" sqref="H10"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="12.28515625" style="10" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="11.7109375" style="13" customWidth="1"/>
+    <col min="3" max="3" width="12.7109375" style="13" customWidth="1"/>
+    <col min="4" max="4" width="8" style="4" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="9.140625" style="4"/>
+    <col min="6" max="6" width="9.85546875" style="4" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="9.140625" style="4"/>
+    <col min="8" max="8" width="8.85546875" style="4" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A1" s="6" t="s">
+        <v>49</v>
+      </c>
+      <c r="B1" s="6" t="s">
+        <v>45</v>
+      </c>
+      <c r="C1" s="6" t="s">
+        <v>46</v>
+      </c>
+      <c r="D1" s="6" t="s">
+        <v>48</v>
+      </c>
+      <c r="E1" s="6" t="s">
+        <v>2</v>
+      </c>
+      <c r="F1" s="6" t="s">
+        <v>4</v>
+      </c>
+      <c r="G1" s="6" t="s">
+        <v>3</v>
+      </c>
+      <c r="H1" s="6" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A2" s="6" t="s">
+        <v>17</v>
+      </c>
+      <c r="B2" s="6" t="s">
+        <v>60</v>
+      </c>
+      <c r="C2" s="6" t="s">
+        <v>59</v>
+      </c>
+      <c r="D2" s="2" t="s">
+        <v>47</v>
+      </c>
+      <c r="E2" s="3" t="s">
+        <v>54</v>
+      </c>
+      <c r="F2" s="3" t="s">
+        <v>67</v>
+      </c>
+      <c r="G2" s="3" t="s">
+        <v>51</v>
+      </c>
+      <c r="H2" s="3" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A3" s="6" t="s">
+        <v>18</v>
+      </c>
+      <c r="B3" s="6" t="s">
+        <v>60</v>
+      </c>
+      <c r="C3" s="6" t="s">
+        <v>59</v>
+      </c>
+      <c r="D3" s="2" t="s">
+        <v>47</v>
+      </c>
+      <c r="E3" s="3" t="s">
+        <v>54</v>
+      </c>
+      <c r="F3" s="3" t="s">
+        <v>67</v>
+      </c>
+      <c r="G3" s="3" t="s">
+        <v>51</v>
+      </c>
+      <c r="H3" s="3" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A4" s="7" t="s">
+        <v>19</v>
+      </c>
+      <c r="B4" s="6" t="s">
+        <v>60</v>
+      </c>
+      <c r="C4" s="6" t="s">
+        <v>59</v>
+      </c>
+      <c r="D4" s="2" t="s">
+        <v>47</v>
+      </c>
+      <c r="E4" s="3" t="s">
+        <v>54</v>
+      </c>
+      <c r="F4" s="3" t="s">
+        <v>67</v>
+      </c>
+      <c r="G4" s="3" t="s">
+        <v>55</v>
+      </c>
+      <c r="H4" s="3" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A5" s="7" t="s">
+        <v>20</v>
+      </c>
+      <c r="B5" s="6" t="s">
+        <v>60</v>
+      </c>
+      <c r="C5" s="6" t="s">
+        <v>59</v>
+      </c>
+      <c r="D5" s="2" t="s">
+        <v>47</v>
+      </c>
+      <c r="E5" s="3" t="s">
+        <v>54</v>
+      </c>
+      <c r="F5" s="3" t="s">
+        <v>67</v>
+      </c>
+      <c r="G5" s="3" t="s">
+        <v>55</v>
+      </c>
+      <c r="H5" s="3" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A6" s="6" t="s">
+        <v>21</v>
+      </c>
+      <c r="B6" s="6" t="s">
+        <v>60</v>
+      </c>
+      <c r="C6" s="6" t="s">
+        <v>59</v>
+      </c>
+      <c r="D6" s="2" t="s">
+        <v>47</v>
+      </c>
+      <c r="E6" s="3" t="s">
+        <v>54</v>
+      </c>
+      <c r="F6" s="3" t="s">
+        <v>54</v>
+      </c>
+      <c r="G6" s="3" t="s">
+        <v>55</v>
+      </c>
+      <c r="H6" s="3" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A7" s="6" t="s">
+        <v>31</v>
+      </c>
+      <c r="B7" s="6" t="s">
+        <v>60</v>
+      </c>
+      <c r="C7" s="6" t="s">
+        <v>59</v>
+      </c>
+      <c r="D7" s="2" t="s">
+        <v>47</v>
+      </c>
+      <c r="E7" s="3" t="s">
+        <v>54</v>
+      </c>
+      <c r="F7" s="3" t="s">
+        <v>54</v>
+      </c>
+      <c r="G7" s="3" t="s">
+        <v>55</v>
+      </c>
+      <c r="H7" s="3" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A8" s="6" t="s">
+        <v>22</v>
+      </c>
+      <c r="B8" s="6" t="s">
+        <v>60</v>
+      </c>
+      <c r="C8" s="6" t="s">
+        <v>59</v>
+      </c>
+      <c r="D8" s="2" t="s">
+        <v>47</v>
+      </c>
+      <c r="E8" s="3" t="s">
+        <v>54</v>
+      </c>
+      <c r="F8" s="3" t="s">
+        <v>67</v>
+      </c>
+      <c r="G8" s="3" t="s">
+        <v>55</v>
+      </c>
+      <c r="H8" s="3" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A9" s="6" t="s">
+        <v>23</v>
+      </c>
+      <c r="B9" s="6" t="s">
+        <v>60</v>
+      </c>
+      <c r="C9" s="6" t="s">
+        <v>59</v>
+      </c>
+      <c r="D9" s="2" t="s">
+        <v>47</v>
+      </c>
+      <c r="E9" s="3" t="s">
+        <v>54</v>
+      </c>
+      <c r="F9" s="3" t="s">
+        <v>67</v>
+      </c>
+      <c r="G9" s="3" t="s">
+        <v>55</v>
+      </c>
+      <c r="H9" s="3" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A10" s="7" t="s">
+        <v>68</v>
+      </c>
+      <c r="B10" s="6" t="s">
+        <v>60</v>
+      </c>
+      <c r="C10" s="6" t="s">
+        <v>59</v>
+      </c>
+      <c r="D10" s="2" t="s">
+        <v>47</v>
+      </c>
+      <c r="E10" s="3" t="s">
+        <v>54</v>
+      </c>
+      <c r="F10" s="3" t="s">
+        <v>54</v>
+      </c>
+      <c r="G10" s="3" t="s">
+        <v>55</v>
+      </c>
+      <c r="H10" s="3" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A11" s="6" t="s">
+        <v>24</v>
+      </c>
+      <c r="B11" s="6" t="s">
+        <v>60</v>
+      </c>
+      <c r="C11" s="6" t="s">
+        <v>59</v>
+      </c>
+      <c r="D11" s="2" t="s">
+        <v>47</v>
+      </c>
+      <c r="E11" s="3" t="s">
+        <v>54</v>
+      </c>
+      <c r="F11" s="3" t="s">
+        <v>54</v>
+      </c>
+      <c r="G11" s="3" t="s">
+        <v>55</v>
+      </c>
+      <c r="H11" s="3" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A12" s="6" t="s">
+        <v>25</v>
+      </c>
+      <c r="B12" s="6" t="s">
+        <v>60</v>
+      </c>
+      <c r="C12" s="6" t="s">
+        <v>59</v>
+      </c>
+      <c r="D12" s="2" t="s">
+        <v>47</v>
+      </c>
+      <c r="E12" s="3" t="s">
+        <v>54</v>
+      </c>
+      <c r="F12" s="3" t="s">
+        <v>67</v>
+      </c>
+      <c r="G12" s="3" t="s">
+        <v>55</v>
+      </c>
+      <c r="H12" s="3" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A13" s="6" t="s">
+        <v>26</v>
+      </c>
+      <c r="B13" s="6" t="s">
+        <v>60</v>
+      </c>
+      <c r="C13" s="6" t="s">
+        <v>59</v>
+      </c>
+      <c r="D13" s="2" t="s">
+        <v>47</v>
+      </c>
+      <c r="E13" s="3" t="s">
+        <v>54</v>
+      </c>
+      <c r="F13" s="3" t="s">
+        <v>67</v>
+      </c>
+      <c r="G13" s="3" t="s">
+        <v>55</v>
+      </c>
+      <c r="H13" s="3" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A14" s="6" t="s">
+        <v>27</v>
+      </c>
+      <c r="B14" s="6" t="s">
+        <v>60</v>
+      </c>
+      <c r="C14" s="6" t="s">
+        <v>59</v>
+      </c>
+      <c r="D14" s="2" t="s">
+        <v>47</v>
+      </c>
+      <c r="E14" s="3" t="s">
+        <v>54</v>
+      </c>
+      <c r="F14" s="3" t="s">
+        <v>67</v>
+      </c>
+      <c r="G14" s="3" t="s">
+        <v>55</v>
+      </c>
+      <c r="H14" s="3" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A15" s="6" t="s">
+        <v>28</v>
+      </c>
+      <c r="B15" s="6" t="s">
+        <v>60</v>
+      </c>
+      <c r="C15" s="6" t="s">
+        <v>59</v>
+      </c>
+      <c r="D15" s="2" t="s">
+        <v>47</v>
+      </c>
+      <c r="E15" s="3" t="s">
+        <v>54</v>
+      </c>
+      <c r="F15" s="3" t="s">
+        <v>54</v>
+      </c>
+      <c r="G15" s="3" t="s">
+        <v>55</v>
+      </c>
+      <c r="H15" s="3" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="16" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A16" s="6" t="s">
+        <v>29</v>
+      </c>
+      <c r="B16" s="6" t="s">
+        <v>60</v>
+      </c>
+      <c r="C16" s="6" t="s">
+        <v>59</v>
+      </c>
+      <c r="D16" s="2" t="s">
+        <v>47</v>
+      </c>
+      <c r="E16" s="3" t="s">
+        <v>54</v>
+      </c>
+      <c r="F16" s="3" t="s">
+        <v>54</v>
+      </c>
+      <c r="G16" s="3" t="s">
+        <v>54</v>
+      </c>
+      <c r="H16" s="3" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="17" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A17" s="6" t="s">
+        <v>30</v>
+      </c>
+      <c r="B17" s="6" t="s">
+        <v>60</v>
+      </c>
+      <c r="C17" s="6" t="s">
+        <v>59</v>
+      </c>
+      <c r="D17" s="2" t="s">
+        <v>47</v>
+      </c>
+      <c r="E17" s="3" t="s">
+        <v>54</v>
+      </c>
+      <c r="F17" s="3" t="s">
+        <v>54</v>
+      </c>
+      <c r="G17" s="3" t="s">
+        <v>55</v>
+      </c>
+      <c r="H17" s="3" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="18" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A18" s="6" t="s">
+        <v>40</v>
+      </c>
+      <c r="B18" s="6" t="s">
+        <v>60</v>
+      </c>
+      <c r="C18" s="6" t="s">
+        <v>59</v>
+      </c>
+      <c r="D18" s="2" t="s">
+        <v>47</v>
+      </c>
+      <c r="E18" s="3" t="s">
+        <v>54</v>
+      </c>
+      <c r="F18" s="3" t="s">
+        <v>67</v>
+      </c>
+      <c r="G18" s="3" t="s">
+        <v>55</v>
+      </c>
+      <c r="H18" s="3" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="19" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A19" s="6" t="s">
+        <v>41</v>
+      </c>
+      <c r="B19" s="6" t="s">
+        <v>60</v>
+      </c>
+      <c r="C19" s="6" t="s">
+        <v>59</v>
+      </c>
+      <c r="D19" s="2" t="s">
+        <v>47</v>
+      </c>
+      <c r="E19" s="3" t="s">
+        <v>54</v>
+      </c>
+      <c r="F19" s="3" t="s">
+        <v>54</v>
+      </c>
+      <c r="G19" s="3" t="s">
+        <v>55</v>
+      </c>
+      <c r="H19" s="3" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="20" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A20" s="6" t="s">
+        <v>42</v>
+      </c>
+      <c r="B20" s="6" t="s">
+        <v>60</v>
+      </c>
+      <c r="C20" s="6" t="s">
+        <v>59</v>
+      </c>
+      <c r="D20" s="2" t="s">
+        <v>47</v>
+      </c>
+      <c r="E20" s="3" t="s">
+        <v>54</v>
+      </c>
+      <c r="F20" s="3" t="s">
+        <v>54</v>
+      </c>
+      <c r="G20" s="3" t="s">
+        <v>55</v>
+      </c>
+      <c r="H20" s="3" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="1048576" spans="8:8" x14ac:dyDescent="0.25">
+      <c r="H1048576" s="3"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I1048576"/>
   <sheetViews>
     <sheetView zoomScale="85" zoomScaleNormal="85" zoomScalePageLayoutView="85" workbookViewId="0">
-      <selection activeCell="N17" sqref="N17"/>
+      <selection sqref="A1:I1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2770,7 +3322,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F20"/>
   <sheetViews>
@@ -3197,7 +3749,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:L23"/>
   <sheetViews>

</xml_diff>

<commit_message>
including processes and fix to databases
</commit_message>
<xml_diff>
--- a/cea/databases/SIN/archetypes/construction_properties.xlsx
+++ b/cea/databases/SIN/archetypes/construction_properties.xlsx
@@ -5,11 +5,11 @@
   <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Gabriel\Documents\GitHub\CEAforArcGIS\cea\databases\SIN\archetypes\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\JimenoF\Documents\Github\CityEnergyAnalyst\cea\databases\SIN\archetypes\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="465" windowWidth="38400" windowHeight="22020" tabRatio="785" firstSheet="1" activeTab="3"/>
+    <workbookView xWindow="0" yWindow="465" windowWidth="38400" windowHeight="22020" tabRatio="785" firstSheet="1" activeTab="4"/>
   </bookViews>
   <sheets>
     <sheet name="ARCHITECTURE" sheetId="3" r:id="rId1"/>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="604" uniqueCount="73">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="603" uniqueCount="72">
   <si>
     <t>Code</t>
   </si>
@@ -129,9 +129,6 @@
     <t>FOODSTORE</t>
   </si>
   <si>
-    <t>Ere_Wm2</t>
-  </si>
-  <si>
     <t>Ed_Wm2</t>
   </si>
   <si>
@@ -231,9 +228,6 @@
     <t>Qhpro_Wm2</t>
   </si>
   <si>
-    <t>Qcpro_Wm2</t>
-  </si>
-  <si>
     <t>T4</t>
   </si>
   <si>
@@ -250,6 +244,9 @@
   </si>
   <si>
     <t>rhum_max_pc</t>
+  </si>
+  <si>
+    <t>Qcre_Wm2</t>
   </si>
 </sst>
 </file>
@@ -776,7 +773,7 @@
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="17" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="14">
+  <cellXfs count="13">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="34" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="17" fillId="33" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -808,7 +805,6 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="16" fillId="34" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="164" fontId="0" fillId="34" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
     <xf numFmtId="49" fontId="0" fillId="34" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -1145,8 +1141,8 @@
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="12" style="10" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="9.7109375" style="13" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="8.7109375" style="13" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="9.7109375" style="12" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="8.7109375" style="12" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="9.28515625" style="4" customWidth="1"/>
     <col min="5" max="5" width="7.140625" style="4" customWidth="1"/>
     <col min="6" max="6" width="10.28515625" style="4" bestFit="1" customWidth="1"/>
@@ -1159,49 +1155,49 @@
   <sheetData>
     <row r="1" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A1" s="6" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="B1" s="6" t="s">
+        <v>44</v>
+      </c>
+      <c r="C1" s="6" t="s">
         <v>45</v>
       </c>
-      <c r="C1" s="6" t="s">
-        <v>46</v>
-      </c>
       <c r="D1" s="6" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="E1" s="6" t="s">
         <v>1</v>
       </c>
       <c r="F1" s="6" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="G1" s="6" t="s">
+        <v>60</v>
+      </c>
+      <c r="H1" s="6" t="s">
         <v>61</v>
       </c>
-      <c r="H1" s="6" t="s">
+      <c r="I1" s="6" t="s">
         <v>62</v>
       </c>
-      <c r="I1" s="6" t="s">
+      <c r="J1" s="6" t="s">
         <v>63</v>
       </c>
-      <c r="J1" s="6" t="s">
-        <v>64</v>
-      </c>
       <c r="K1" s="6" t="s">
+        <v>42</v>
+      </c>
+      <c r="L1" s="6" t="s">
         <v>43</v>
       </c>
-      <c r="L1" s="6" t="s">
-        <v>44</v>
-      </c>
       <c r="M1" s="6" t="s">
+        <v>35</v>
+      </c>
+      <c r="N1" s="6" t="s">
+        <v>37</v>
+      </c>
+      <c r="O1" s="6" t="s">
         <v>36</v>
-      </c>
-      <c r="N1" s="6" t="s">
-        <v>38</v>
-      </c>
-      <c r="O1" s="6" t="s">
-        <v>37</v>
       </c>
       <c r="P1" s="6" t="s">
         <v>6</v>
@@ -1212,13 +1208,13 @@
         <v>17</v>
       </c>
       <c r="B2" s="6" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="C2" s="6" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="D2" s="2" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="E2" s="3">
         <v>0.25</v>
@@ -1239,22 +1235,22 @@
         <v>0.28999999999999998</v>
       </c>
       <c r="K2" s="3" t="s">
+        <v>50</v>
+      </c>
+      <c r="L2" s="3" t="s">
+        <v>54</v>
+      </c>
+      <c r="M2" s="3" t="s">
+        <v>55</v>
+      </c>
+      <c r="N2" s="3" t="s">
         <v>51</v>
       </c>
-      <c r="L2" s="3" t="s">
-        <v>55</v>
-      </c>
-      <c r="M2" s="3" t="s">
-        <v>56</v>
-      </c>
-      <c r="N2" s="3" t="s">
-        <v>52</v>
-      </c>
       <c r="O2" s="3" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="P2" s="3" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="R2" s="11"/>
     </row>
@@ -1263,13 +1259,13 @@
         <v>18</v>
       </c>
       <c r="B3" s="6" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="C3" s="6" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="D3" s="2" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="E3" s="3">
         <v>0.25</v>
@@ -1290,22 +1286,22 @@
         <v>0.28999999999999998</v>
       </c>
       <c r="K3" s="3" t="s">
+        <v>50</v>
+      </c>
+      <c r="L3" s="3" t="s">
+        <v>54</v>
+      </c>
+      <c r="M3" s="3" t="s">
+        <v>55</v>
+      </c>
+      <c r="N3" s="3" t="s">
         <v>51</v>
       </c>
-      <c r="L3" s="3" t="s">
-        <v>55</v>
-      </c>
-      <c r="M3" s="3" t="s">
-        <v>56</v>
-      </c>
-      <c r="N3" s="3" t="s">
-        <v>52</v>
-      </c>
       <c r="O3" s="3" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="P3" s="3" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
     </row>
     <row r="4" spans="1:18" x14ac:dyDescent="0.25">
@@ -1313,13 +1309,13 @@
         <v>19</v>
       </c>
       <c r="B4" s="6" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="C4" s="6" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="D4" s="2" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="E4" s="3">
         <v>0.84</v>
@@ -1340,22 +1336,22 @@
         <v>0.35</v>
       </c>
       <c r="K4" s="3" t="s">
+        <v>50</v>
+      </c>
+      <c r="L4" s="3" t="s">
+        <v>49</v>
+      </c>
+      <c r="M4" s="3" t="s">
+        <v>57</v>
+      </c>
+      <c r="N4" s="3" t="s">
         <v>51</v>
       </c>
-      <c r="L4" s="3" t="s">
-        <v>50</v>
-      </c>
-      <c r="M4" s="3" t="s">
-        <v>58</v>
-      </c>
-      <c r="N4" s="3" t="s">
+      <c r="O4" s="3" t="s">
         <v>52</v>
       </c>
-      <c r="O4" s="3" t="s">
-        <v>53</v>
-      </c>
       <c r="P4" s="3" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
     </row>
     <row r="5" spans="1:18" x14ac:dyDescent="0.25">
@@ -1363,13 +1359,13 @@
         <v>20</v>
       </c>
       <c r="B5" s="6" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="C5" s="6" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="D5" s="2" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="E5" s="3">
         <v>0.84</v>
@@ -1390,22 +1386,22 @@
         <v>0.35</v>
       </c>
       <c r="K5" s="3" t="s">
+        <v>50</v>
+      </c>
+      <c r="L5" s="3" t="s">
+        <v>49</v>
+      </c>
+      <c r="M5" s="3" t="s">
+        <v>57</v>
+      </c>
+      <c r="N5" s="3" t="s">
         <v>51</v>
       </c>
-      <c r="L5" s="3" t="s">
-        <v>50</v>
-      </c>
-      <c r="M5" s="3" t="s">
-        <v>58</v>
-      </c>
-      <c r="N5" s="3" t="s">
+      <c r="O5" s="3" t="s">
         <v>52</v>
       </c>
-      <c r="O5" s="3" t="s">
-        <v>53</v>
-      </c>
       <c r="P5" s="3" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
     </row>
     <row r="6" spans="1:18" x14ac:dyDescent="0.25">
@@ -1413,13 +1409,13 @@
         <v>21</v>
       </c>
       <c r="B6" s="6" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="C6" s="6" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="D6" s="2" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="E6" s="3">
         <v>0.84</v>
@@ -1440,22 +1436,22 @@
         <v>0.35</v>
       </c>
       <c r="K6" s="3" t="s">
+        <v>50</v>
+      </c>
+      <c r="L6" s="3" t="s">
+        <v>49</v>
+      </c>
+      <c r="M6" s="3" t="s">
+        <v>57</v>
+      </c>
+      <c r="N6" s="3" t="s">
         <v>51</v>
       </c>
-      <c r="L6" s="3" t="s">
-        <v>50</v>
-      </c>
-      <c r="M6" s="3" t="s">
-        <v>58</v>
-      </c>
-      <c r="N6" s="3" t="s">
+      <c r="O6" s="3" t="s">
         <v>52</v>
       </c>
-      <c r="O6" s="3" t="s">
-        <v>53</v>
-      </c>
       <c r="P6" s="3" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
     </row>
     <row r="7" spans="1:18" x14ac:dyDescent="0.25">
@@ -1463,13 +1459,13 @@
         <v>31</v>
       </c>
       <c r="B7" s="6" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="C7" s="6" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="D7" s="2" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="E7" s="3">
         <v>0.84</v>
@@ -1490,22 +1486,22 @@
         <v>0</v>
       </c>
       <c r="K7" s="3" t="s">
+        <v>50</v>
+      </c>
+      <c r="L7" s="3" t="s">
+        <v>49</v>
+      </c>
+      <c r="M7" s="3" t="s">
+        <v>57</v>
+      </c>
+      <c r="N7" s="3" t="s">
         <v>51</v>
       </c>
-      <c r="L7" s="3" t="s">
-        <v>50</v>
-      </c>
-      <c r="M7" s="3" t="s">
-        <v>58</v>
-      </c>
-      <c r="N7" s="3" t="s">
+      <c r="O7" s="3" t="s">
         <v>52</v>
       </c>
-      <c r="O7" s="3" t="s">
-        <v>53</v>
-      </c>
       <c r="P7" s="3" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
     </row>
     <row r="8" spans="1:18" x14ac:dyDescent="0.25">
@@ -1513,13 +1509,13 @@
         <v>22</v>
       </c>
       <c r="B8" s="6" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="C8" s="6" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="D8" s="2" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="E8" s="3">
         <v>0.84</v>
@@ -1540,22 +1536,22 @@
         <v>0.35</v>
       </c>
       <c r="K8" s="3" t="s">
+        <v>50</v>
+      </c>
+      <c r="L8" s="3" t="s">
+        <v>49</v>
+      </c>
+      <c r="M8" s="3" t="s">
+        <v>57</v>
+      </c>
+      <c r="N8" s="3" t="s">
         <v>51</v>
       </c>
-      <c r="L8" s="3" t="s">
-        <v>50</v>
-      </c>
-      <c r="M8" s="3" t="s">
-        <v>58</v>
-      </c>
-      <c r="N8" s="3" t="s">
+      <c r="O8" s="3" t="s">
         <v>52</v>
       </c>
-      <c r="O8" s="3" t="s">
-        <v>53</v>
-      </c>
       <c r="P8" s="3" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
     </row>
     <row r="9" spans="1:18" x14ac:dyDescent="0.25">
@@ -1563,13 +1559,13 @@
         <v>23</v>
       </c>
       <c r="B9" s="6" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="C9" s="6" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="D9" s="2" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="E9" s="3">
         <v>0.7</v>
@@ -1590,36 +1586,36 @@
         <v>0.1</v>
       </c>
       <c r="K9" s="3" t="s">
+        <v>50</v>
+      </c>
+      <c r="L9" s="3" t="s">
+        <v>49</v>
+      </c>
+      <c r="M9" s="3" t="s">
+        <v>57</v>
+      </c>
+      <c r="N9" s="3" t="s">
         <v>51</v>
       </c>
-      <c r="L9" s="3" t="s">
-        <v>50</v>
-      </c>
-      <c r="M9" s="3" t="s">
-        <v>58</v>
-      </c>
-      <c r="N9" s="3" t="s">
+      <c r="O9" s="3" t="s">
         <v>52</v>
       </c>
-      <c r="O9" s="3" t="s">
-        <v>53</v>
-      </c>
       <c r="P9" s="3" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
     </row>
     <row r="10" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A10" s="6" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="B10" s="6" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="C10" s="6" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="D10" s="2" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="E10" s="3">
         <v>0.67</v>
@@ -1640,22 +1636,22 @@
         <v>0.35</v>
       </c>
       <c r="K10" s="3" t="s">
+        <v>50</v>
+      </c>
+      <c r="L10" s="3" t="s">
+        <v>49</v>
+      </c>
+      <c r="M10" s="3" t="s">
+        <v>57</v>
+      </c>
+      <c r="N10" s="3" t="s">
         <v>51</v>
       </c>
-      <c r="L10" s="3" t="s">
-        <v>50</v>
-      </c>
-      <c r="M10" s="3" t="s">
-        <v>58</v>
-      </c>
-      <c r="N10" s="3" t="s">
+      <c r="O10" s="3" t="s">
         <v>52</v>
       </c>
-      <c r="O10" s="3" t="s">
-        <v>53</v>
-      </c>
       <c r="P10" s="3" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
     </row>
     <row r="11" spans="1:18" x14ac:dyDescent="0.25">
@@ -1663,13 +1659,13 @@
         <v>24</v>
       </c>
       <c r="B11" s="6" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="C11" s="6" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="D11" s="2" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="E11" s="3">
         <v>0.67</v>
@@ -1690,22 +1686,22 @@
         <v>0.35</v>
       </c>
       <c r="K11" s="3" t="s">
+        <v>50</v>
+      </c>
+      <c r="L11" s="3" t="s">
+        <v>49</v>
+      </c>
+      <c r="M11" s="3" t="s">
+        <v>56</v>
+      </c>
+      <c r="N11" s="3" t="s">
         <v>51</v>
       </c>
-      <c r="L11" s="3" t="s">
-        <v>50</v>
-      </c>
-      <c r="M11" s="3" t="s">
-        <v>57</v>
-      </c>
-      <c r="N11" s="3" t="s">
+      <c r="O11" s="3" t="s">
         <v>52</v>
       </c>
-      <c r="O11" s="3" t="s">
-        <v>53</v>
-      </c>
       <c r="P11" s="3" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
     </row>
     <row r="12" spans="1:18" x14ac:dyDescent="0.25">
@@ -1713,13 +1709,13 @@
         <v>25</v>
       </c>
       <c r="B12" s="6" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="C12" s="6" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="D12" s="2" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="E12" s="3">
         <v>0.84</v>
@@ -1740,22 +1736,22 @@
         <v>0.35</v>
       </c>
       <c r="K12" s="3" t="s">
+        <v>50</v>
+      </c>
+      <c r="L12" s="3" t="s">
+        <v>49</v>
+      </c>
+      <c r="M12" s="3" t="s">
+        <v>57</v>
+      </c>
+      <c r="N12" s="3" t="s">
         <v>51</v>
       </c>
-      <c r="L12" s="3" t="s">
-        <v>50</v>
-      </c>
-      <c r="M12" s="3" t="s">
-        <v>58</v>
-      </c>
-      <c r="N12" s="3" t="s">
+      <c r="O12" s="3" t="s">
         <v>52</v>
       </c>
-      <c r="O12" s="3" t="s">
-        <v>53</v>
-      </c>
       <c r="P12" s="3" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
     </row>
     <row r="13" spans="1:18" x14ac:dyDescent="0.25">
@@ -1763,13 +1759,13 @@
         <v>26</v>
       </c>
       <c r="B13" s="6" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="C13" s="6" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="D13" s="2" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="E13" s="3">
         <v>0.67</v>
@@ -1790,22 +1786,22 @@
         <v>0.35</v>
       </c>
       <c r="K13" s="3" t="s">
+        <v>50</v>
+      </c>
+      <c r="L13" s="3" t="s">
+        <v>49</v>
+      </c>
+      <c r="M13" s="3" t="s">
+        <v>56</v>
+      </c>
+      <c r="N13" s="3" t="s">
         <v>51</v>
       </c>
-      <c r="L13" s="3" t="s">
-        <v>50</v>
-      </c>
-      <c r="M13" s="3" t="s">
-        <v>57</v>
-      </c>
-      <c r="N13" s="3" t="s">
+      <c r="O13" s="3" t="s">
         <v>52</v>
       </c>
-      <c r="O13" s="3" t="s">
-        <v>53</v>
-      </c>
       <c r="P13" s="3" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
     </row>
     <row r="14" spans="1:18" x14ac:dyDescent="0.25">
@@ -1813,13 +1809,13 @@
         <v>27</v>
       </c>
       <c r="B14" s="6" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="C14" s="6" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="D14" s="2" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="E14" s="3">
         <v>0</v>
@@ -1840,22 +1836,22 @@
         <v>0.35</v>
       </c>
       <c r="K14" s="3" t="s">
+        <v>50</v>
+      </c>
+      <c r="L14" s="3" t="s">
+        <v>49</v>
+      </c>
+      <c r="M14" s="3" t="s">
+        <v>57</v>
+      </c>
+      <c r="N14" s="3" t="s">
         <v>51</v>
       </c>
-      <c r="L14" s="3" t="s">
-        <v>50</v>
-      </c>
-      <c r="M14" s="3" t="s">
-        <v>58</v>
-      </c>
-      <c r="N14" s="3" t="s">
-        <v>52</v>
-      </c>
       <c r="O14" s="3" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="P14" s="3" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
     </row>
     <row r="15" spans="1:18" x14ac:dyDescent="0.25">
@@ -1863,13 +1859,13 @@
         <v>28</v>
       </c>
       <c r="B15" s="6" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="C15" s="6" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="D15" s="2" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="E15" s="3">
         <v>1</v>
@@ -1890,22 +1886,22 @@
         <v>0</v>
       </c>
       <c r="K15" s="3" t="s">
+        <v>50</v>
+      </c>
+      <c r="L15" s="3" t="s">
+        <v>49</v>
+      </c>
+      <c r="M15" s="3" t="s">
+        <v>57</v>
+      </c>
+      <c r="N15" s="3" t="s">
         <v>51</v>
       </c>
-      <c r="L15" s="3" t="s">
-        <v>50</v>
-      </c>
-      <c r="M15" s="3" t="s">
-        <v>58</v>
-      </c>
-      <c r="N15" s="3" t="s">
+      <c r="O15" s="3" t="s">
         <v>52</v>
       </c>
-      <c r="O15" s="3" t="s">
-        <v>53</v>
-      </c>
       <c r="P15" s="3" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
     </row>
     <row r="16" spans="1:18" x14ac:dyDescent="0.25">
@@ -1913,13 +1909,13 @@
         <v>29</v>
       </c>
       <c r="B16" s="6" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="C16" s="6" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="D16" s="2" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="E16" s="3">
         <v>0</v>
@@ -1940,22 +1936,22 @@
         <v>0.5</v>
       </c>
       <c r="K16" s="3" t="s">
+        <v>50</v>
+      </c>
+      <c r="L16" s="3" t="s">
+        <v>52</v>
+      </c>
+      <c r="M16" s="3" t="s">
+        <v>49</v>
+      </c>
+      <c r="N16" s="3" t="s">
         <v>51</v>
       </c>
-      <c r="L16" s="3" t="s">
-        <v>53</v>
-      </c>
-      <c r="M16" s="3" t="s">
-        <v>50</v>
-      </c>
-      <c r="N16" s="3" t="s">
-        <v>52</v>
-      </c>
       <c r="O16" s="3" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="P16" s="3" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
     </row>
     <row r="17" spans="1:16" x14ac:dyDescent="0.25">
@@ -1963,13 +1959,13 @@
         <v>30</v>
       </c>
       <c r="B17" s="6" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="C17" s="6" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="D17" s="2" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="E17" s="3">
         <v>1</v>
@@ -1990,36 +1986,36 @@
         <v>0</v>
       </c>
       <c r="K17" s="3" t="s">
+        <v>50</v>
+      </c>
+      <c r="L17" s="3" t="s">
+        <v>49</v>
+      </c>
+      <c r="M17" s="3" t="s">
+        <v>49</v>
+      </c>
+      <c r="N17" s="3" t="s">
         <v>51</v>
       </c>
-      <c r="L17" s="3" t="s">
-        <v>50</v>
-      </c>
-      <c r="M17" s="3" t="s">
-        <v>50</v>
-      </c>
-      <c r="N17" s="3" t="s">
+      <c r="O17" s="3" t="s">
         <v>52</v>
       </c>
-      <c r="O17" s="3" t="s">
-        <v>53</v>
-      </c>
       <c r="P17" s="3" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
     </row>
     <row r="18" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A18" s="6" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="B18" s="6" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="C18" s="6" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="D18" s="2" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="E18" s="3">
         <v>0.67</v>
@@ -2040,36 +2036,36 @@
         <v>0.35</v>
       </c>
       <c r="K18" s="3" t="s">
+        <v>50</v>
+      </c>
+      <c r="L18" s="3" t="s">
+        <v>49</v>
+      </c>
+      <c r="M18" s="3" t="s">
+        <v>56</v>
+      </c>
+      <c r="N18" s="3" t="s">
         <v>51</v>
       </c>
-      <c r="L18" s="3" t="s">
-        <v>50</v>
-      </c>
-      <c r="M18" s="3" t="s">
-        <v>57</v>
-      </c>
-      <c r="N18" s="3" t="s">
+      <c r="O18" s="3" t="s">
         <v>52</v>
       </c>
-      <c r="O18" s="3" t="s">
-        <v>53</v>
-      </c>
       <c r="P18" s="3" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
     </row>
     <row r="19" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A19" s="6" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="B19" s="6" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="C19" s="6" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="D19" s="2" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="E19" s="3">
         <v>0.67</v>
@@ -2090,36 +2086,36 @@
         <v>0.35</v>
       </c>
       <c r="K19" s="3" t="s">
+        <v>50</v>
+      </c>
+      <c r="L19" s="3" t="s">
+        <v>49</v>
+      </c>
+      <c r="M19" s="3" t="s">
+        <v>56</v>
+      </c>
+      <c r="N19" s="3" t="s">
         <v>51</v>
       </c>
-      <c r="L19" s="3" t="s">
-        <v>50</v>
-      </c>
-      <c r="M19" s="3" t="s">
-        <v>57</v>
-      </c>
-      <c r="N19" s="3" t="s">
+      <c r="O19" s="3" t="s">
         <v>52</v>
       </c>
-      <c r="O19" s="3" t="s">
-        <v>53</v>
-      </c>
       <c r="P19" s="3" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
     </row>
     <row r="20" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A20" s="6" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="B20" s="6" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="C20" s="6" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="D20" s="2" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="E20" s="3">
         <v>0.67</v>
@@ -2140,22 +2136,22 @@
         <v>0.35</v>
       </c>
       <c r="K20" s="3" t="s">
+        <v>50</v>
+      </c>
+      <c r="L20" s="3" t="s">
+        <v>49</v>
+      </c>
+      <c r="M20" s="3" t="s">
+        <v>56</v>
+      </c>
+      <c r="N20" s="3" t="s">
         <v>51</v>
       </c>
-      <c r="L20" s="3" t="s">
-        <v>50</v>
-      </c>
-      <c r="M20" s="3" t="s">
-        <v>57</v>
-      </c>
-      <c r="N20" s="3" t="s">
+      <c r="O20" s="3" t="s">
         <v>52</v>
       </c>
-      <c r="O20" s="3" t="s">
-        <v>53</v>
-      </c>
       <c r="P20" s="3" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
     </row>
   </sheetData>
@@ -2178,8 +2174,8 @@
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="12.28515625" style="10" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="11.7109375" style="13" customWidth="1"/>
-    <col min="3" max="3" width="12.7109375" style="13" customWidth="1"/>
+    <col min="2" max="2" width="11.7109375" style="12" customWidth="1"/>
+    <col min="3" max="3" width="12.7109375" style="12" customWidth="1"/>
     <col min="4" max="4" width="8" style="4" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="9.140625" style="4"/>
     <col min="6" max="6" width="9.85546875" style="4" bestFit="1" customWidth="1"/>
@@ -2189,16 +2185,16 @@
   <sheetData>
     <row r="1" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A1" s="6" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="B1" s="6" t="s">
+        <v>44</v>
+      </c>
+      <c r="C1" s="6" t="s">
         <v>45</v>
       </c>
-      <c r="C1" s="6" t="s">
-        <v>46</v>
-      </c>
       <c r="D1" s="6" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="E1" s="6" t="s">
         <v>2</v>
@@ -2210,7 +2206,7 @@
         <v>3</v>
       </c>
       <c r="H1" s="6" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.25">
@@ -2218,25 +2214,25 @@
         <v>17</v>
       </c>
       <c r="B2" s="6" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="C2" s="6" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="D2" s="2" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="E2" s="3" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="F2" s="3" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="G2" s="3" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="H2" s="3" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.25">
@@ -2244,25 +2240,25 @@
         <v>18</v>
       </c>
       <c r="B3" s="6" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="C3" s="6" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="D3" s="2" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="E3" s="3" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="F3" s="3" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="G3" s="3" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="H3" s="3" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.25">
@@ -2270,25 +2266,25 @@
         <v>19</v>
       </c>
       <c r="B4" s="6" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="C4" s="6" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="D4" s="2" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="E4" s="3" t="s">
+        <v>53</v>
+      </c>
+      <c r="F4" s="3" t="s">
+        <v>65</v>
+      </c>
+      <c r="G4" s="3" t="s">
         <v>54</v>
       </c>
-      <c r="F4" s="3" t="s">
-        <v>67</v>
-      </c>
-      <c r="G4" s="3" t="s">
-        <v>55</v>
-      </c>
       <c r="H4" s="3" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.25">
@@ -2296,25 +2292,25 @@
         <v>20</v>
       </c>
       <c r="B5" s="6" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="C5" s="6" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="D5" s="2" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="E5" s="3" t="s">
+        <v>53</v>
+      </c>
+      <c r="F5" s="3" t="s">
+        <v>65</v>
+      </c>
+      <c r="G5" s="3" t="s">
         <v>54</v>
       </c>
-      <c r="F5" s="3" t="s">
-        <v>67</v>
-      </c>
-      <c r="G5" s="3" t="s">
-        <v>55</v>
-      </c>
       <c r="H5" s="3" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.25">
@@ -2322,25 +2318,25 @@
         <v>21</v>
       </c>
       <c r="B6" s="6" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="C6" s="6" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="D6" s="2" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="E6" s="3" t="s">
+        <v>53</v>
+      </c>
+      <c r="F6" s="3" t="s">
+        <v>53</v>
+      </c>
+      <c r="G6" s="3" t="s">
         <v>54</v>
       </c>
-      <c r="F6" s="3" t="s">
-        <v>54</v>
-      </c>
-      <c r="G6" s="3" t="s">
-        <v>55</v>
-      </c>
       <c r="H6" s="3" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.25">
@@ -2348,25 +2344,25 @@
         <v>31</v>
       </c>
       <c r="B7" s="6" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="C7" s="6" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="D7" s="2" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="E7" s="3" t="s">
+        <v>53</v>
+      </c>
+      <c r="F7" s="3" t="s">
+        <v>53</v>
+      </c>
+      <c r="G7" s="3" t="s">
         <v>54</v>
       </c>
-      <c r="F7" s="3" t="s">
-        <v>54</v>
-      </c>
-      <c r="G7" s="3" t="s">
-        <v>55</v>
-      </c>
       <c r="H7" s="3" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.25">
@@ -2374,25 +2370,25 @@
         <v>22</v>
       </c>
       <c r="B8" s="6" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="C8" s="6" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="D8" s="2" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="E8" s="3" t="s">
+        <v>53</v>
+      </c>
+      <c r="F8" s="3" t="s">
+        <v>65</v>
+      </c>
+      <c r="G8" s="3" t="s">
         <v>54</v>
       </c>
-      <c r="F8" s="3" t="s">
-        <v>67</v>
-      </c>
-      <c r="G8" s="3" t="s">
-        <v>55</v>
-      </c>
       <c r="H8" s="3" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.25">
@@ -2400,51 +2396,51 @@
         <v>23</v>
       </c>
       <c r="B9" s="6" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="C9" s="6" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="D9" s="2" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="E9" s="3" t="s">
+        <v>53</v>
+      </c>
+      <c r="F9" s="3" t="s">
+        <v>65</v>
+      </c>
+      <c r="G9" s="3" t="s">
         <v>54</v>
       </c>
-      <c r="F9" s="3" t="s">
-        <v>67</v>
-      </c>
-      <c r="G9" s="3" t="s">
-        <v>55</v>
-      </c>
       <c r="H9" s="3" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A10" s="7" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="B10" s="6" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="C10" s="6" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="D10" s="2" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="E10" s="3" t="s">
+        <v>53</v>
+      </c>
+      <c r="F10" s="3" t="s">
+        <v>53</v>
+      </c>
+      <c r="G10" s="3" t="s">
         <v>54</v>
       </c>
-      <c r="F10" s="3" t="s">
-        <v>54</v>
-      </c>
-      <c r="G10" s="3" t="s">
-        <v>55</v>
-      </c>
       <c r="H10" s="3" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
     </row>
     <row r="11" spans="1:8" x14ac:dyDescent="0.25">
@@ -2452,25 +2448,25 @@
         <v>24</v>
       </c>
       <c r="B11" s="6" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="C11" s="6" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="D11" s="2" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="E11" s="3" t="s">
+        <v>53</v>
+      </c>
+      <c r="F11" s="3" t="s">
+        <v>53</v>
+      </c>
+      <c r="G11" s="3" t="s">
         <v>54</v>
       </c>
-      <c r="F11" s="3" t="s">
-        <v>54</v>
-      </c>
-      <c r="G11" s="3" t="s">
-        <v>55</v>
-      </c>
       <c r="H11" s="3" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
     </row>
     <row r="12" spans="1:8" x14ac:dyDescent="0.25">
@@ -2478,25 +2474,25 @@
         <v>25</v>
       </c>
       <c r="B12" s="6" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="C12" s="6" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="D12" s="2" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="E12" s="3" t="s">
+        <v>53</v>
+      </c>
+      <c r="F12" s="3" t="s">
+        <v>65</v>
+      </c>
+      <c r="G12" s="3" t="s">
         <v>54</v>
       </c>
-      <c r="F12" s="3" t="s">
-        <v>67</v>
-      </c>
-      <c r="G12" s="3" t="s">
-        <v>55</v>
-      </c>
       <c r="H12" s="3" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
     </row>
     <row r="13" spans="1:8" x14ac:dyDescent="0.25">
@@ -2504,25 +2500,25 @@
         <v>26</v>
       </c>
       <c r="B13" s="6" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="C13" s="6" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="D13" s="2" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="E13" s="3" t="s">
+        <v>53</v>
+      </c>
+      <c r="F13" s="3" t="s">
+        <v>65</v>
+      </c>
+      <c r="G13" s="3" t="s">
         <v>54</v>
       </c>
-      <c r="F13" s="3" t="s">
-        <v>67</v>
-      </c>
-      <c r="G13" s="3" t="s">
-        <v>55</v>
-      </c>
       <c r="H13" s="3" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
     </row>
     <row r="14" spans="1:8" x14ac:dyDescent="0.25">
@@ -2530,25 +2526,25 @@
         <v>27</v>
       </c>
       <c r="B14" s="6" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="C14" s="6" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="D14" s="2" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="E14" s="3" t="s">
+        <v>53</v>
+      </c>
+      <c r="F14" s="3" t="s">
+        <v>65</v>
+      </c>
+      <c r="G14" s="3" t="s">
         <v>54</v>
       </c>
-      <c r="F14" s="3" t="s">
-        <v>67</v>
-      </c>
-      <c r="G14" s="3" t="s">
-        <v>55</v>
-      </c>
       <c r="H14" s="3" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
     </row>
     <row r="15" spans="1:8" x14ac:dyDescent="0.25">
@@ -2556,25 +2552,25 @@
         <v>28</v>
       </c>
       <c r="B15" s="6" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="C15" s="6" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="D15" s="2" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="E15" s="3" t="s">
+        <v>53</v>
+      </c>
+      <c r="F15" s="3" t="s">
+        <v>53</v>
+      </c>
+      <c r="G15" s="3" t="s">
         <v>54</v>
       </c>
-      <c r="F15" s="3" t="s">
-        <v>54</v>
-      </c>
-      <c r="G15" s="3" t="s">
-        <v>55</v>
-      </c>
       <c r="H15" s="3" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
     </row>
     <row r="16" spans="1:8" x14ac:dyDescent="0.25">
@@ -2582,25 +2578,25 @@
         <v>29</v>
       </c>
       <c r="B16" s="6" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="C16" s="6" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="D16" s="2" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="E16" s="3" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="F16" s="3" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="G16" s="3" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="H16" s="3" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
     </row>
     <row r="17" spans="1:8" x14ac:dyDescent="0.25">
@@ -2608,103 +2604,103 @@
         <v>30</v>
       </c>
       <c r="B17" s="6" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="C17" s="6" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="D17" s="2" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="E17" s="3" t="s">
+        <v>53</v>
+      </c>
+      <c r="F17" s="3" t="s">
+        <v>53</v>
+      </c>
+      <c r="G17" s="3" t="s">
         <v>54</v>
       </c>
-      <c r="F17" s="3" t="s">
-        <v>54</v>
-      </c>
-      <c r="G17" s="3" t="s">
-        <v>55</v>
-      </c>
       <c r="H17" s="3" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
     </row>
     <row r="18" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A18" s="6" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="B18" s="6" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="C18" s="6" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="D18" s="2" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="E18" s="3" t="s">
+        <v>53</v>
+      </c>
+      <c r="F18" s="3" t="s">
+        <v>65</v>
+      </c>
+      <c r="G18" s="3" t="s">
         <v>54</v>
       </c>
-      <c r="F18" s="3" t="s">
-        <v>67</v>
-      </c>
-      <c r="G18" s="3" t="s">
-        <v>55</v>
-      </c>
       <c r="H18" s="3" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
     </row>
     <row r="19" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A19" s="6" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="B19" s="6" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="C19" s="6" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="D19" s="2" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="E19" s="3" t="s">
+        <v>53</v>
+      </c>
+      <c r="F19" s="3" t="s">
+        <v>53</v>
+      </c>
+      <c r="G19" s="3" t="s">
         <v>54</v>
       </c>
-      <c r="F19" s="3" t="s">
-        <v>54</v>
-      </c>
-      <c r="G19" s="3" t="s">
-        <v>55</v>
-      </c>
       <c r="H19" s="3" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
     </row>
     <row r="20" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A20" s="6" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="B20" s="6" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="C20" s="6" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="D20" s="2" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="E20" s="3" t="s">
+        <v>53</v>
+      </c>
+      <c r="F20" s="3" t="s">
+        <v>53</v>
+      </c>
+      <c r="G20" s="3" t="s">
         <v>54</v>
       </c>
-      <c r="F20" s="3" t="s">
-        <v>54</v>
-      </c>
-      <c r="G20" s="3" t="s">
-        <v>55</v>
-      </c>
       <c r="H20" s="3" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
     </row>
     <row r="1048576" spans="8:8" x14ac:dyDescent="0.25">
@@ -2726,8 +2722,8 @@
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="12.28515625" style="10" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="11.7109375" style="13" customWidth="1"/>
-    <col min="3" max="3" width="12.7109375" style="13" customWidth="1"/>
+    <col min="2" max="2" width="11.7109375" style="12" customWidth="1"/>
+    <col min="3" max="3" width="12.7109375" style="12" customWidth="1"/>
     <col min="4" max="4" width="8" style="4" bestFit="1" customWidth="1"/>
     <col min="5" max="6" width="9.140625" style="4"/>
     <col min="7" max="7" width="9.85546875" style="4" bestFit="1" customWidth="1"/>
@@ -2738,16 +2734,16 @@
   <sheetData>
     <row r="1" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A1" s="6" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="B1" s="6" t="s">
+        <v>44</v>
+      </c>
+      <c r="C1" s="6" t="s">
         <v>45</v>
       </c>
-      <c r="C1" s="6" t="s">
-        <v>46</v>
-      </c>
       <c r="D1" s="6" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="E1" s="6" t="s">
         <v>2</v>
@@ -2762,7 +2758,7 @@
         <v>5</v>
       </c>
       <c r="I1" s="6" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.25">
@@ -2770,28 +2766,28 @@
         <v>17</v>
       </c>
       <c r="B2" s="6" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="C2" s="6" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="D2" s="2" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="E2" s="3" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="F2" s="3" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="G2" s="3" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="H2" s="3" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="I2" s="3" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.25">
@@ -2799,28 +2795,28 @@
         <v>18</v>
       </c>
       <c r="B3" s="6" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="C3" s="6" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="D3" s="2" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="E3" s="3" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="F3" s="3" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="G3" s="3" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="H3" s="3" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="I3" s="3" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.25">
@@ -2828,28 +2824,28 @@
         <v>19</v>
       </c>
       <c r="B4" s="6" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="C4" s="6" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="D4" s="2" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="E4" s="3" t="s">
+        <v>53</v>
+      </c>
+      <c r="F4" s="3" t="s">
         <v>54</v>
       </c>
-      <c r="F4" s="3" t="s">
-        <v>55</v>
-      </c>
       <c r="G4" s="3" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="H4" s="3" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="I4" s="3" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.25">
@@ -2857,28 +2853,28 @@
         <v>20</v>
       </c>
       <c r="B5" s="6" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="C5" s="6" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="D5" s="2" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="E5" s="3" t="s">
+        <v>53</v>
+      </c>
+      <c r="F5" s="3" t="s">
         <v>54</v>
       </c>
-      <c r="F5" s="3" t="s">
-        <v>55</v>
-      </c>
       <c r="G5" s="3" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="H5" s="3" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="I5" s="3" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.25">
@@ -2886,28 +2882,28 @@
         <v>21</v>
       </c>
       <c r="B6" s="6" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="C6" s="6" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="D6" s="2" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="E6" s="3" t="s">
+        <v>53</v>
+      </c>
+      <c r="F6" s="3" t="s">
         <v>54</v>
       </c>
-      <c r="F6" s="3" t="s">
-        <v>55</v>
-      </c>
       <c r="G6" s="3" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="H6" s="3" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="I6" s="3" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.25">
@@ -2915,28 +2911,28 @@
         <v>31</v>
       </c>
       <c r="B7" s="6" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="C7" s="6" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="D7" s="2" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="E7" s="3" t="s">
+        <v>53</v>
+      </c>
+      <c r="F7" s="3" t="s">
         <v>54</v>
       </c>
-      <c r="F7" s="3" t="s">
-        <v>55</v>
-      </c>
       <c r="G7" s="3" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="H7" s="3" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="I7" s="3" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
     </row>
     <row r="8" spans="1:9" x14ac:dyDescent="0.25">
@@ -2944,28 +2940,28 @@
         <v>22</v>
       </c>
       <c r="B8" s="6" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="C8" s="6" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="D8" s="2" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="E8" s="3" t="s">
+        <v>53</v>
+      </c>
+      <c r="F8" s="3" t="s">
         <v>54</v>
       </c>
-      <c r="F8" s="3" t="s">
-        <v>55</v>
-      </c>
       <c r="G8" s="3" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="H8" s="3" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="I8" s="3" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
     </row>
     <row r="9" spans="1:9" x14ac:dyDescent="0.25">
@@ -2973,57 +2969,57 @@
         <v>23</v>
       </c>
       <c r="B9" s="6" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="C9" s="6" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="D9" s="2" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="E9" s="3" t="s">
+        <v>53</v>
+      </c>
+      <c r="F9" s="3" t="s">
         <v>54</v>
       </c>
-      <c r="F9" s="3" t="s">
-        <v>55</v>
-      </c>
       <c r="G9" s="3" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="H9" s="3" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="I9" s="3" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
     </row>
     <row r="10" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A10" s="7" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="B10" s="6" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="C10" s="6" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="D10" s="2" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="E10" s="3" t="s">
+        <v>53</v>
+      </c>
+      <c r="F10" s="3" t="s">
         <v>54</v>
       </c>
-      <c r="F10" s="3" t="s">
-        <v>55</v>
-      </c>
       <c r="G10" s="3" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="H10" s="3" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="I10" s="3" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
     </row>
     <row r="11" spans="1:9" x14ac:dyDescent="0.25">
@@ -3031,28 +3027,28 @@
         <v>24</v>
       </c>
       <c r="B11" s="6" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="C11" s="6" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="D11" s="2" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="E11" s="3" t="s">
+        <v>53</v>
+      </c>
+      <c r="F11" s="3" t="s">
         <v>54</v>
       </c>
-      <c r="F11" s="3" t="s">
-        <v>55</v>
-      </c>
       <c r="G11" s="3" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="H11" s="3" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="I11" s="3" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
     </row>
     <row r="12" spans="1:9" x14ac:dyDescent="0.25">
@@ -3060,28 +3056,28 @@
         <v>25</v>
       </c>
       <c r="B12" s="6" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="C12" s="6" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="D12" s="2" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="E12" s="3" t="s">
+        <v>53</v>
+      </c>
+      <c r="F12" s="3" t="s">
         <v>54</v>
       </c>
-      <c r="F12" s="3" t="s">
-        <v>55</v>
-      </c>
       <c r="G12" s="3" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="H12" s="3" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="I12" s="3" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
     </row>
     <row r="13" spans="1:9" x14ac:dyDescent="0.25">
@@ -3089,28 +3085,28 @@
         <v>26</v>
       </c>
       <c r="B13" s="6" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="C13" s="6" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="D13" s="2" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="E13" s="3" t="s">
+        <v>53</v>
+      </c>
+      <c r="F13" s="3" t="s">
         <v>54</v>
       </c>
-      <c r="F13" s="3" t="s">
-        <v>55</v>
-      </c>
       <c r="G13" s="3" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="H13" s="3" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="I13" s="3" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
     </row>
     <row r="14" spans="1:9" x14ac:dyDescent="0.25">
@@ -3118,28 +3114,28 @@
         <v>27</v>
       </c>
       <c r="B14" s="6" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="C14" s="6" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="D14" s="2" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="E14" s="3" t="s">
+        <v>53</v>
+      </c>
+      <c r="F14" s="3" t="s">
         <v>54</v>
       </c>
-      <c r="F14" s="3" t="s">
-        <v>55</v>
-      </c>
       <c r="G14" s="3" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="H14" s="3" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="I14" s="3" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
     </row>
     <row r="15" spans="1:9" x14ac:dyDescent="0.25">
@@ -3147,28 +3143,28 @@
         <v>28</v>
       </c>
       <c r="B15" s="6" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="C15" s="6" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="D15" s="2" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="E15" s="3" t="s">
+        <v>53</v>
+      </c>
+      <c r="F15" s="3" t="s">
         <v>54</v>
       </c>
-      <c r="F15" s="3" t="s">
-        <v>55</v>
-      </c>
       <c r="G15" s="3" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="H15" s="3" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="I15" s="3" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
     </row>
     <row r="16" spans="1:9" x14ac:dyDescent="0.25">
@@ -3176,28 +3172,28 @@
         <v>29</v>
       </c>
       <c r="B16" s="6" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="C16" s="6" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="D16" s="2" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="E16" s="3" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="F16" s="3" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="G16" s="3" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="H16" s="3" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="I16" s="3" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
     </row>
     <row r="17" spans="1:9" x14ac:dyDescent="0.25">
@@ -3205,115 +3201,115 @@
         <v>30</v>
       </c>
       <c r="B17" s="6" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="C17" s="6" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="D17" s="2" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="E17" s="3" t="s">
+        <v>53</v>
+      </c>
+      <c r="F17" s="3" t="s">
         <v>54</v>
       </c>
-      <c r="F17" s="3" t="s">
-        <v>55</v>
-      </c>
       <c r="G17" s="3" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="H17" s="3" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="I17" s="3" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
     </row>
     <row r="18" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A18" s="6" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="B18" s="6" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="C18" s="6" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="D18" s="2" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="E18" s="3" t="s">
+        <v>53</v>
+      </c>
+      <c r="F18" s="3" t="s">
         <v>54</v>
       </c>
-      <c r="F18" s="3" t="s">
-        <v>55</v>
-      </c>
       <c r="G18" s="3" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="H18" s="3" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="I18" s="3" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
     </row>
     <row r="19" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A19" s="6" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="B19" s="6" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="C19" s="6" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="D19" s="2" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="E19" s="3" t="s">
+        <v>53</v>
+      </c>
+      <c r="F19" s="3" t="s">
         <v>54</v>
       </c>
-      <c r="F19" s="3" t="s">
-        <v>55</v>
-      </c>
       <c r="G19" s="3" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="H19" s="3" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="I19" s="3" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
     </row>
     <row r="20" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A20" s="6" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="B20" s="6" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="C20" s="6" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="D20" s="2" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="E20" s="3" t="s">
+        <v>53</v>
+      </c>
+      <c r="F20" s="3" t="s">
         <v>54</v>
       </c>
-      <c r="F20" s="3" t="s">
-        <v>55</v>
-      </c>
       <c r="G20" s="3" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="H20" s="3" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="I20" s="3" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
     </row>
     <row r="1048576" spans="8:8" x14ac:dyDescent="0.25">
@@ -3332,7 +3328,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H20"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" zoomScalePageLayoutView="85" workbookViewId="0">
+    <sheetView zoomScale="85" zoomScaleNormal="85" zoomScalePageLayoutView="85" workbookViewId="0">
       <selection activeCell="H2" sqref="H2"/>
     </sheetView>
   </sheetViews>
@@ -3358,19 +3354,19 @@
         <v>8</v>
       </c>
       <c r="D1" s="6" t="s">
+        <v>33</v>
+      </c>
+      <c r="E1" s="6" t="s">
         <v>34</v>
-      </c>
-      <c r="E1" s="6" t="s">
-        <v>35</v>
       </c>
       <c r="F1" s="6" t="s">
         <v>7</v>
       </c>
       <c r="G1" s="6" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="H1" s="6" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.25">
@@ -3584,7 +3580,7 @@
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A10" s="6" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="B10" s="8">
         <v>24</v>
@@ -3792,7 +3788,7 @@
     </row>
     <row r="18" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A18" s="6" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="B18" s="8">
         <v>24</v>
@@ -3819,7 +3815,7 @@
     </row>
     <row r="19" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A19" s="6" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="B19" s="8">
         <v>24</v>
@@ -3845,7 +3841,7 @@
     </row>
     <row r="20" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A20" s="6" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="B20" s="8">
         <v>24</v>
@@ -3877,10 +3873,10 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:L23"/>
+  <dimension ref="A1:K20"/>
   <sheetViews>
-    <sheetView zoomScale="85" zoomScaleNormal="85" zoomScalePageLayoutView="85" workbookViewId="0">
-      <selection activeCell="Q19" sqref="Q19"/>
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" zoomScalePageLayoutView="85" workbookViewId="0">
+      <selection activeCell="N17" sqref="N17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3889,16 +3885,15 @@
     <col min="2" max="3" width="8.28515625" style="1" customWidth="1"/>
     <col min="4" max="4" width="10.28515625" style="1" customWidth="1"/>
     <col min="5" max="5" width="8.140625" style="1" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="10.28515625" style="1" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="9.28515625" style="1" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="10.28515625" style="1" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="11.140625" style="1" customWidth="1"/>
-    <col min="10" max="10" width="9.7109375" style="1" customWidth="1"/>
-    <col min="11" max="11" width="11.140625" style="1" bestFit="1" customWidth="1"/>
+    <col min="6" max="7" width="10.28515625" style="1" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="11.140625" style="1" customWidth="1"/>
+    <col min="9" max="9" width="9.7109375" style="1" customWidth="1"/>
+    <col min="10" max="10" width="11.140625" style="1" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="10.7109375" style="1" bestFit="1" customWidth="1"/>
     <col min="12" max="16384" width="9.140625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A1" s="6" t="s">
         <v>0</v>
       </c>
@@ -3921,22 +3916,19 @@
         <v>32</v>
       </c>
       <c r="H1" s="6" t="s">
-        <v>33</v>
+        <v>15</v>
       </c>
       <c r="I1" s="6" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="J1" s="6" t="s">
-        <v>16</v>
+        <v>64</v>
       </c>
       <c r="K1" s="6" t="s">
-        <v>65</v>
-      </c>
-      <c r="L1" s="6" t="s">
-        <v>66</v>
-      </c>
-    </row>
-    <row r="2" spans="1:12" x14ac:dyDescent="0.25">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A2" s="6" t="s">
         <v>17</v>
       </c>
@@ -3955,26 +3947,23 @@
       <c r="F2" s="5">
         <v>0</v>
       </c>
-      <c r="G2" s="8">
-        <v>0</v>
-      </c>
-      <c r="H2" s="5">
-        <v>0</v>
+      <c r="G2" s="5">
+        <v>0</v>
+      </c>
+      <c r="H2" s="8">
+        <v>40</v>
       </c>
       <c r="I2" s="8">
-        <v>40</v>
-      </c>
-      <c r="J2" s="8">
         <v>80</v>
       </c>
+      <c r="J2" s="5">
+        <v>0</v>
+      </c>
       <c r="K2" s="5">
         <v>0</v>
       </c>
-      <c r="L2" s="5">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="3" spans="1:12" x14ac:dyDescent="0.25">
+    </row>
+    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A3" s="6" t="s">
         <v>18</v>
       </c>
@@ -3993,26 +3982,23 @@
       <c r="F3" s="8">
         <v>0</v>
       </c>
-      <c r="G3" s="8">
-        <v>0</v>
-      </c>
-      <c r="H3" s="5">
-        <v>0</v>
+      <c r="G3" s="5">
+        <v>0</v>
+      </c>
+      <c r="H3" s="8">
+        <v>40</v>
       </c>
       <c r="I3" s="8">
-        <v>40</v>
-      </c>
-      <c r="J3" s="8">
         <v>80</v>
       </c>
+      <c r="J3" s="5">
+        <v>0</v>
+      </c>
       <c r="K3" s="5">
         <v>0</v>
       </c>
-      <c r="L3" s="5">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="4" spans="1:12" x14ac:dyDescent="0.25">
+    </row>
+    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A4" s="7" t="s">
         <v>19</v>
       </c>
@@ -4031,26 +4017,23 @@
       <c r="F4" s="8">
         <v>0</v>
       </c>
-      <c r="G4" s="8">
-        <v>0</v>
-      </c>
-      <c r="H4" s="5">
-        <v>0</v>
+      <c r="G4" s="5">
+        <v>0</v>
+      </c>
+      <c r="H4" s="8">
+        <v>40</v>
       </c>
       <c r="I4" s="8">
-        <v>40</v>
-      </c>
-      <c r="J4" s="8">
         <v>80</v>
       </c>
+      <c r="J4" s="5">
+        <v>0</v>
+      </c>
       <c r="K4" s="5">
         <v>0</v>
       </c>
-      <c r="L4" s="5">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="5" spans="1:12" x14ac:dyDescent="0.25">
+    </row>
+    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A5" s="6" t="s">
         <v>20</v>
       </c>
@@ -4069,26 +4052,23 @@
       <c r="F5" s="8">
         <v>0</v>
       </c>
-      <c r="G5" s="8">
-        <v>0</v>
-      </c>
-      <c r="H5" s="5">
+      <c r="G5" s="5">
+        <v>0</v>
+      </c>
+      <c r="H5" s="8">
         <v>0</v>
       </c>
       <c r="I5" s="8">
-        <v>0</v>
-      </c>
-      <c r="J5" s="8">
         <v>20</v>
       </c>
+      <c r="J5" s="5">
+        <v>0</v>
+      </c>
       <c r="K5" s="5">
         <v>0</v>
       </c>
-      <c r="L5" s="5">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="6" spans="1:12" x14ac:dyDescent="0.25">
+    </row>
+    <row r="6" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A6" s="6" t="s">
         <v>21</v>
       </c>
@@ -4107,26 +4087,23 @@
       <c r="F6" s="8">
         <v>0</v>
       </c>
-      <c r="G6" s="8">
-        <v>0</v>
-      </c>
-      <c r="H6" s="5">
-        <v>0</v>
+      <c r="G6" s="5">
+        <v>0</v>
+      </c>
+      <c r="H6" s="8">
+        <v>2</v>
       </c>
       <c r="I6" s="8">
-        <v>2</v>
-      </c>
-      <c r="J6" s="8">
         <v>4</v>
       </c>
+      <c r="J6" s="5">
+        <v>0</v>
+      </c>
       <c r="K6" s="5">
         <v>0</v>
       </c>
-      <c r="L6" s="5">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="7" spans="1:12" x14ac:dyDescent="0.25">
+    </row>
+    <row r="7" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A7" s="6" t="s">
         <v>31</v>
       </c>
@@ -4145,26 +4122,23 @@
       <c r="F7" s="8">
         <v>0</v>
       </c>
-      <c r="G7" s="8">
-        <v>0</v>
-      </c>
-      <c r="H7" s="5">
-        <v>0</v>
+      <c r="G7" s="5">
+        <v>0</v>
+      </c>
+      <c r="H7" s="8">
+        <v>2</v>
       </c>
       <c r="I7" s="8">
-        <v>2</v>
-      </c>
-      <c r="J7" s="8">
         <v>4</v>
       </c>
+      <c r="J7" s="5">
+        <v>0</v>
+      </c>
       <c r="K7" s="5">
         <v>0</v>
       </c>
-      <c r="L7" s="5">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="8" spans="1:12" x14ac:dyDescent="0.25">
+    </row>
+    <row r="8" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A8" s="6" t="s">
         <v>22</v>
       </c>
@@ -4183,26 +4157,23 @@
       <c r="F8" s="8">
         <v>0</v>
       </c>
-      <c r="G8" s="8">
-        <v>0</v>
-      </c>
-      <c r="H8" s="5">
-        <v>0</v>
+      <c r="G8" s="5">
+        <v>0</v>
+      </c>
+      <c r="H8" s="8">
+        <v>8</v>
       </c>
       <c r="I8" s="8">
-        <v>8</v>
-      </c>
-      <c r="J8" s="8">
         <v>16</v>
       </c>
+      <c r="J8" s="5">
+        <v>0</v>
+      </c>
       <c r="K8" s="5">
         <v>0</v>
       </c>
-      <c r="L8" s="5">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="9" spans="1:12" x14ac:dyDescent="0.25">
+    </row>
+    <row r="9" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A9" s="6" t="s">
         <v>23</v>
       </c>
@@ -4221,28 +4192,25 @@
       <c r="F9" s="8">
         <v>16.5</v>
       </c>
-      <c r="G9" s="8">
-        <v>0</v>
-      </c>
-      <c r="H9" s="5">
-        <v>0</v>
+      <c r="G9" s="5">
+        <v>0</v>
+      </c>
+      <c r="H9" s="8">
+        <v>10</v>
       </c>
       <c r="I9" s="8">
-        <v>10</v>
-      </c>
-      <c r="J9" s="8">
         <v>20</v>
       </c>
+      <c r="J9" s="5">
+        <v>0</v>
+      </c>
       <c r="K9" s="5">
         <v>0</v>
       </c>
-      <c r="L9" s="5">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="10" spans="1:12" x14ac:dyDescent="0.25">
+    </row>
+    <row r="10" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A10" s="6" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="B10" s="8">
         <v>70</v>
@@ -4259,26 +4227,23 @@
       <c r="F10" s="8">
         <v>0</v>
       </c>
-      <c r="G10" s="8">
-        <v>0</v>
-      </c>
-      <c r="H10" s="5">
+      <c r="G10" s="5">
+        <v>0</v>
+      </c>
+      <c r="H10" s="8">
         <v>0</v>
       </c>
       <c r="I10" s="8">
-        <v>0</v>
-      </c>
-      <c r="J10" s="8">
         <v>20</v>
       </c>
+      <c r="J10" s="5">
+        <v>0</v>
+      </c>
       <c r="K10" s="5">
         <v>0</v>
       </c>
-      <c r="L10" s="5">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="11" spans="1:12" x14ac:dyDescent="0.25">
+    </row>
+    <row r="11" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A11" s="6" t="s">
         <v>24</v>
       </c>
@@ -4297,26 +4262,23 @@
       <c r="F11" s="8">
         <v>0</v>
       </c>
-      <c r="G11" s="8">
-        <v>0</v>
-      </c>
-      <c r="H11" s="5">
+      <c r="G11" s="5">
+        <v>0</v>
+      </c>
+      <c r="H11" s="8">
         <v>0</v>
       </c>
       <c r="I11" s="8">
-        <v>0</v>
-      </c>
-      <c r="J11" s="8">
         <v>4</v>
       </c>
+      <c r="J11" s="5">
+        <v>0</v>
+      </c>
       <c r="K11" s="5">
         <v>0</v>
       </c>
-      <c r="L11" s="5">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="12" spans="1:12" x14ac:dyDescent="0.25">
+    </row>
+    <row r="12" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A12" s="6" t="s">
         <v>25</v>
       </c>
@@ -4335,26 +4297,23 @@
       <c r="F12" s="8">
         <v>0</v>
       </c>
-      <c r="G12" s="8">
-        <v>0</v>
-      </c>
-      <c r="H12" s="5">
+      <c r="G12" s="5">
+        <v>0</v>
+      </c>
+      <c r="H12" s="8">
         <v>0</v>
       </c>
       <c r="I12" s="8">
-        <v>0</v>
-      </c>
-      <c r="J12" s="8">
         <v>80</v>
       </c>
+      <c r="J12" s="5">
+        <v>0</v>
+      </c>
       <c r="K12" s="5">
         <v>0</v>
       </c>
-      <c r="L12" s="5">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="13" spans="1:12" x14ac:dyDescent="0.25">
+    </row>
+    <row r="13" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A13" s="6" t="s">
         <v>26</v>
       </c>
@@ -4373,26 +4332,23 @@
       <c r="F13" s="8">
         <v>0</v>
       </c>
-      <c r="G13" s="8">
-        <v>0</v>
-      </c>
-      <c r="H13" s="5">
-        <v>0</v>
+      <c r="G13" s="5">
+        <v>0</v>
+      </c>
+      <c r="H13" s="8">
+        <v>40</v>
       </c>
       <c r="I13" s="8">
-        <v>40</v>
-      </c>
-      <c r="J13" s="8">
         <v>80</v>
       </c>
+      <c r="J13" s="5">
+        <v>0</v>
+      </c>
       <c r="K13" s="5">
         <v>0</v>
       </c>
-      <c r="L13" s="5">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="14" spans="1:12" x14ac:dyDescent="0.25">
+    </row>
+    <row r="14" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A14" s="6" t="s">
         <v>27</v>
       </c>
@@ -4411,26 +4367,23 @@
       <c r="F14" s="8">
         <v>0</v>
       </c>
-      <c r="G14" s="8">
-        <v>0</v>
-      </c>
-      <c r="H14" s="5">
+      <c r="G14" s="5">
+        <v>0</v>
+      </c>
+      <c r="H14" s="8">
         <v>0</v>
       </c>
       <c r="I14" s="8">
-        <v>0</v>
-      </c>
-      <c r="J14" s="8">
         <v>360</v>
       </c>
+      <c r="J14" s="5">
+        <v>0</v>
+      </c>
       <c r="K14" s="5">
         <v>0</v>
       </c>
-      <c r="L14" s="5">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="15" spans="1:12" x14ac:dyDescent="0.25">
+    </row>
+    <row r="15" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A15" s="6" t="s">
         <v>28</v>
       </c>
@@ -4450,25 +4403,22 @@
         <v>0</v>
       </c>
       <c r="G15" s="8">
-        <v>0</v>
+        <v>500</v>
       </c>
       <c r="H15" s="8">
-        <v>500</v>
+        <v>0</v>
       </c>
       <c r="I15" s="8">
         <v>0</v>
       </c>
-      <c r="J15" s="8">
+      <c r="J15" s="5">
         <v>0</v>
       </c>
       <c r="K15" s="5">
         <v>0</v>
       </c>
-      <c r="L15" s="5">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="16" spans="1:12" x14ac:dyDescent="0.25">
+    </row>
+    <row r="16" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A16" s="6" t="s">
         <v>29</v>
       </c>
@@ -4487,26 +4437,23 @@
       <c r="F16" s="8">
         <v>0</v>
       </c>
-      <c r="G16" s="8">
-        <v>0</v>
-      </c>
-      <c r="H16" s="5">
+      <c r="G16" s="5">
+        <v>0</v>
+      </c>
+      <c r="H16" s="8">
         <v>0</v>
       </c>
       <c r="I16" s="8">
         <v>0</v>
       </c>
-      <c r="J16" s="8">
+      <c r="J16" s="5">
         <v>0</v>
       </c>
       <c r="K16" s="5">
         <v>0</v>
       </c>
-      <c r="L16" s="5">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="17" spans="1:12" x14ac:dyDescent="0.25">
+    </row>
+    <row r="17" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A17" s="6" t="s">
         <v>30</v>
       </c>
@@ -4525,28 +4472,25 @@
       <c r="F17" s="8">
         <v>0</v>
       </c>
-      <c r="G17" s="8">
-        <v>5.6</v>
-      </c>
-      <c r="H17" s="5">
+      <c r="G17" s="5">
+        <v>0</v>
+      </c>
+      <c r="H17" s="8">
         <v>0</v>
       </c>
       <c r="I17" s="8">
         <v>0</v>
       </c>
-      <c r="J17" s="8">
+      <c r="J17" s="5">
         <v>0</v>
       </c>
       <c r="K17" s="5">
-        <v>0</v>
-      </c>
-      <c r="L17" s="5">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="18" spans="1:12" x14ac:dyDescent="0.25">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="18" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A18" s="6" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="B18" s="8">
         <f>B12</f>
@@ -4566,28 +4510,25 @@
         <f>F9</f>
         <v>16.5</v>
       </c>
-      <c r="G18" s="8">
-        <v>0</v>
-      </c>
-      <c r="H18" s="5">
-        <v>0</v>
+      <c r="G18" s="5">
+        <v>0</v>
+      </c>
+      <c r="H18" s="8">
+        <v>10</v>
       </c>
       <c r="I18" s="8">
-        <v>10</v>
-      </c>
-      <c r="J18" s="8">
         <v>20</v>
       </c>
+      <c r="J18" s="5">
+        <v>0</v>
+      </c>
       <c r="K18" s="5">
         <v>0</v>
       </c>
-      <c r="L18" s="5">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="19" spans="1:12" x14ac:dyDescent="0.25">
+    </row>
+    <row r="19" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A19" s="6" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="B19" s="8">
         <v>70</v>
@@ -4604,28 +4545,25 @@
       <c r="F19" s="8">
         <v>0</v>
       </c>
-      <c r="G19" s="8">
-        <v>0</v>
-      </c>
-      <c r="H19" s="5">
+      <c r="G19" s="5">
+        <v>0</v>
+      </c>
+      <c r="H19" s="8">
         <v>0</v>
       </c>
       <c r="I19" s="8">
-        <v>0</v>
-      </c>
-      <c r="J19" s="8">
         <v>4</v>
       </c>
+      <c r="J19" s="5">
+        <v>0</v>
+      </c>
       <c r="K19" s="5">
         <v>0</v>
       </c>
-      <c r="L19" s="5">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="20" spans="1:12" x14ac:dyDescent="0.25">
+    </row>
+    <row r="20" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A20" s="6" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="B20" s="8">
         <v>70</v>
@@ -4642,27 +4580,21 @@
       <c r="F20" s="8">
         <v>0</v>
       </c>
-      <c r="G20" s="8">
-        <v>0</v>
-      </c>
-      <c r="H20" s="5">
+      <c r="G20" s="5">
+        <v>0</v>
+      </c>
+      <c r="H20" s="8">
         <v>0</v>
       </c>
       <c r="I20" s="8">
-        <v>0</v>
-      </c>
-      <c r="J20" s="8">
         <v>4</v>
       </c>
+      <c r="J20" s="5">
+        <v>0</v>
+      </c>
       <c r="K20" s="5">
         <v>0</v>
       </c>
-      <c r="L20" s="5">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="23" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="G23" s="12"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
use new SG wall types "T8" and "T7" based on BCA ETTV example
</commit_message>
<xml_diff>
--- a/cea/databases/SIN/archetypes/construction_properties.xlsx
+++ b/cea/databases/SIN/archetypes/construction_properties.xlsx
@@ -5,11 +5,11 @@
   <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\JimenoF\Documents\Github\CityEnergyAnalyst\cea\databases\SIN\archetypes\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Gabriel\Documents\GitHub\CEAforArcGIS\cea\databases\SIN\archetypes\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="465" windowWidth="38400" windowHeight="22020" tabRatio="785" firstSheet="1" activeTab="4"/>
+    <workbookView xWindow="0" yWindow="465" windowWidth="38400" windowHeight="22020" tabRatio="785"/>
   </bookViews>
   <sheets>
     <sheet name="ARCHITECTURE" sheetId="3" r:id="rId1"/>
@@ -1131,11 +1131,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:R20"/>
   <sheetViews>
-    <sheetView zoomScale="85" zoomScaleNormal="85" zoomScalePageLayoutView="85" workbookViewId="0">
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" zoomScalePageLayoutView="85" workbookViewId="0">
       <pane xSplit="4" ySplit="1" topLeftCell="E2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="D1" sqref="D1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="F3" sqref="F3"/>
+      <selection pane="bottomRight" activeCell="O20" sqref="O20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1247,7 +1247,7 @@
         <v>51</v>
       </c>
       <c r="O2" s="3" t="s">
-        <v>50</v>
+        <v>55</v>
       </c>
       <c r="P2" s="3" t="s">
         <v>49</v>
@@ -1298,7 +1298,7 @@
         <v>51</v>
       </c>
       <c r="O3" s="3" t="s">
-        <v>50</v>
+        <v>55</v>
       </c>
       <c r="P3" s="3" t="s">
         <v>49</v>
@@ -1348,7 +1348,7 @@
         <v>51</v>
       </c>
       <c r="O4" s="3" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="P4" s="3" t="s">
         <v>49</v>
@@ -1398,7 +1398,7 @@
         <v>51</v>
       </c>
       <c r="O5" s="3" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="P5" s="3" t="s">
         <v>49</v>
@@ -1448,7 +1448,7 @@
         <v>51</v>
       </c>
       <c r="O6" s="3" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="P6" s="3" t="s">
         <v>49</v>
@@ -1498,7 +1498,7 @@
         <v>51</v>
       </c>
       <c r="O7" s="3" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="P7" s="3" t="s">
         <v>49</v>
@@ -1548,7 +1548,7 @@
         <v>51</v>
       </c>
       <c r="O8" s="3" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="P8" s="3" t="s">
         <v>49</v>
@@ -1598,7 +1598,7 @@
         <v>51</v>
       </c>
       <c r="O9" s="3" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="P9" s="3" t="s">
         <v>49</v>
@@ -1648,7 +1648,7 @@
         <v>51</v>
       </c>
       <c r="O10" s="3" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="P10" s="3" t="s">
         <v>49</v>
@@ -1698,7 +1698,7 @@
         <v>51</v>
       </c>
       <c r="O11" s="3" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="P11" s="3" t="s">
         <v>49</v>
@@ -1748,7 +1748,7 @@
         <v>51</v>
       </c>
       <c r="O12" s="3" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="P12" s="3" t="s">
         <v>49</v>
@@ -1798,7 +1798,7 @@
         <v>51</v>
       </c>
       <c r="O13" s="3" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="P13" s="3" t="s">
         <v>49</v>
@@ -1848,7 +1848,7 @@
         <v>51</v>
       </c>
       <c r="O14" s="3" t="s">
-        <v>50</v>
+        <v>55</v>
       </c>
       <c r="P14" s="3" t="s">
         <v>53</v>
@@ -1898,7 +1898,7 @@
         <v>51</v>
       </c>
       <c r="O15" s="3" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="P15" s="3" t="s">
         <v>49</v>
@@ -1948,7 +1948,7 @@
         <v>51</v>
       </c>
       <c r="O16" s="3" t="s">
-        <v>50</v>
+        <v>55</v>
       </c>
       <c r="P16" s="3" t="s">
         <v>53</v>
@@ -1998,7 +1998,7 @@
         <v>51</v>
       </c>
       <c r="O17" s="3" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="P17" s="3" t="s">
         <v>49</v>
@@ -2048,7 +2048,7 @@
         <v>51</v>
       </c>
       <c r="O18" s="3" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="P18" s="3" t="s">
         <v>49</v>
@@ -2098,7 +2098,7 @@
         <v>51</v>
       </c>
       <c r="O19" s="3" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="P19" s="3" t="s">
         <v>49</v>
@@ -2148,7 +2148,7 @@
         <v>51</v>
       </c>
       <c r="O20" s="3" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="P20" s="3" t="s">
         <v>49</v>
@@ -3875,7 +3875,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:K20"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" zoomScalePageLayoutView="85" workbookViewId="0">
+    <sheetView zoomScale="85" zoomScaleNormal="85" zoomScalePageLayoutView="85" workbookViewId="0">
       <selection activeCell="N17" sqref="N17"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
higher WWR of 0.59 (sinberbest benchmark office) for SG Office, Retail, Restaurant
</commit_message>
<xml_diff>
--- a/cea/databases/SIN/archetypes/construction_properties.xlsx
+++ b/cea/databases/SIN/archetypes/construction_properties.xlsx
@@ -1135,7 +1135,7 @@
       <pane xSplit="4" ySplit="1" topLeftCell="E2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="D1" sqref="D1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="O20" sqref="O20"/>
+      <selection pane="bottomRight" activeCell="G8" sqref="G8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1374,16 +1374,16 @@
         <v>0</v>
       </c>
       <c r="G5" s="3">
-        <v>0.35</v>
+        <v>0.59</v>
       </c>
       <c r="H5" s="3">
-        <v>0.35</v>
+        <v>0.59</v>
       </c>
       <c r="I5" s="3">
-        <v>0.35</v>
+        <v>0.59</v>
       </c>
       <c r="J5" s="3">
-        <v>0.35</v>
+        <v>0.59</v>
       </c>
       <c r="K5" s="3" t="s">
         <v>50</v>
@@ -1424,16 +1424,16 @@
         <v>0</v>
       </c>
       <c r="G6" s="3">
-        <v>0.35</v>
+        <v>0.59</v>
       </c>
       <c r="H6" s="3">
-        <v>0.35</v>
+        <v>0.59</v>
       </c>
       <c r="I6" s="3">
-        <v>0.35</v>
+        <v>0.59</v>
       </c>
       <c r="J6" s="3">
-        <v>0.35</v>
+        <v>0.59</v>
       </c>
       <c r="K6" s="3" t="s">
         <v>50</v>
@@ -1524,16 +1524,16 @@
         <v>0</v>
       </c>
       <c r="G8" s="3">
-        <v>0.35</v>
+        <v>0.59</v>
       </c>
       <c r="H8" s="3">
-        <v>0.35</v>
+        <v>0.59</v>
       </c>
       <c r="I8" s="3">
-        <v>0.35</v>
+        <v>0.59</v>
       </c>
       <c r="J8" s="3">
-        <v>0.35</v>
+        <v>0.59</v>
       </c>
       <c r="K8" s="3" t="s">
         <v>50</v>

</xml_diff>

<commit_message>
lower installed appliance and lighting power density in SG
- Residential -50%
- Office -30%
</commit_message>
<xml_diff>
--- a/cea/databases/SIN/archetypes/construction_properties.xlsx
+++ b/cea/databases/SIN/archetypes/construction_properties.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="465" windowWidth="38400" windowHeight="22020" tabRatio="785"/>
+    <workbookView xWindow="0" yWindow="465" windowWidth="38400" windowHeight="22020" tabRatio="785" activeTab="4"/>
   </bookViews>
   <sheets>
     <sheet name="ARCHITECTURE" sheetId="3" r:id="rId1"/>
@@ -1131,7 +1131,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:R20"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" zoomScalePageLayoutView="85" workbookViewId="0">
+    <sheetView zoomScale="85" zoomScaleNormal="85" zoomScalePageLayoutView="85" workbookViewId="0">
       <pane xSplit="4" ySplit="1" topLeftCell="E2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="D1" sqref="D1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
@@ -3875,8 +3875,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:K20"/>
   <sheetViews>
-    <sheetView zoomScale="85" zoomScaleNormal="85" zoomScalePageLayoutView="85" workbookViewId="0">
-      <selection activeCell="N17" sqref="N17"/>
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" zoomScalePageLayoutView="85" workbookViewId="0">
+      <selection activeCell="D6" sqref="D6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3939,10 +3939,10 @@
         <v>80</v>
       </c>
       <c r="D2" s="8">
-        <v>5.5</v>
+        <v>2</v>
       </c>
       <c r="E2" s="8">
-        <v>10.5</v>
+        <v>5</v>
       </c>
       <c r="F2" s="5">
         <v>0</v>
@@ -3974,10 +3974,10 @@
         <v>80</v>
       </c>
       <c r="D3" s="5">
-        <v>5.5</v>
+        <v>2</v>
       </c>
       <c r="E3" s="5">
-        <v>10.52</v>
+        <v>5</v>
       </c>
       <c r="F3" s="8">
         <v>0</v>
@@ -4044,10 +4044,10 @@
         <v>80</v>
       </c>
       <c r="D5" s="8">
-        <v>15</v>
+        <v>11</v>
       </c>
       <c r="E5" s="8">
-        <v>14</v>
+        <v>10</v>
       </c>
       <c r="F5" s="8">
         <v>0</v>

</xml_diff>

<commit_message>
fixing occupancy and construciton properties
</commit_message>
<xml_diff>
--- a/cea/databases/SIN/archetypes/construction_properties.xlsx
+++ b/cea/databases/SIN/archetypes/construction_properties.xlsx
@@ -5,11 +5,11 @@
   <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Gabriel\Documents\GitHub\CEAforArcGIS\cea\databases\SIN\archetypes\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\JimenoF\Documents\Github\CityEnergyAnalyst\cea\databases\SIN\archetypes\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="465" windowWidth="38400" windowHeight="22020" tabRatio="785" activeTab="4"/>
+    <workbookView xWindow="0" yWindow="465" windowWidth="38400" windowHeight="22020" tabRatio="785" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="ARCHITECTURE" sheetId="3" r:id="rId1"/>
@@ -3328,8 +3328,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H20"/>
   <sheetViews>
-    <sheetView zoomScale="85" zoomScaleNormal="85" zoomScalePageLayoutView="85" workbookViewId="0">
-      <selection activeCell="H2" sqref="H2"/>
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" zoomScalePageLayoutView="85" workbookViewId="0">
+      <selection activeCell="Q11" sqref="Q11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3374,13 +3374,13 @@
         <v>17</v>
       </c>
       <c r="B2" s="8">
-        <v>24</v>
+        <v>28</v>
       </c>
       <c r="C2" s="5">
         <v>10</v>
       </c>
       <c r="D2" s="8">
-        <v>24</v>
+        <v>27</v>
       </c>
       <c r="E2" s="5">
         <v>10</v>
@@ -3400,13 +3400,13 @@
         <v>18</v>
       </c>
       <c r="B3" s="8">
-        <v>24</v>
+        <v>28</v>
       </c>
       <c r="C3" s="5">
         <v>10</v>
       </c>
       <c r="D3" s="8">
-        <v>24</v>
+        <v>27</v>
       </c>
       <c r="E3" s="5">
         <v>10</v>
@@ -3875,7 +3875,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:K20"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" zoomScalePageLayoutView="85" workbookViewId="0">
+    <sheetView zoomScale="85" zoomScaleNormal="85" zoomScalePageLayoutView="85" workbookViewId="0">
       <selection activeCell="D6" sqref="D6"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
Add 'Es' to construction archetypes
</commit_message>
<xml_diff>
--- a/cea/databases/SIN/archetypes/construction_properties.xlsx
+++ b/cea/databases/SIN/archetypes/construction_properties.xlsx
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="604" uniqueCount="73">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="605" uniqueCount="74">
   <si>
     <t>Code</t>
   </si>
@@ -250,6 +250,9 @@
   </si>
   <si>
     <t>Ns</t>
+  </si>
+  <si>
+    <t>Es</t>
   </si>
 </sst>
 </file>
@@ -1132,13 +1135,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:S20"/>
+  <dimension ref="A1:T20"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" zoomScalePageLayoutView="85" workbookViewId="0">
       <pane xSplit="4" ySplit="1" topLeftCell="E2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="D1" sqref="D1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight"/>
+      <selection pane="bottomRight" activeCell="E2" sqref="E2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.1640625" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -1147,16 +1150,16 @@
     <col min="2" max="2" width="9.6640625" style="12" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="8.6640625" style="12" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="9.33203125" style="4" customWidth="1"/>
-    <col min="5" max="6" width="7.1640625" style="4" customWidth="1"/>
-    <col min="7" max="7" width="10.33203125" style="4" bestFit="1" customWidth="1"/>
-    <col min="8" max="11" width="10.83203125" style="4" customWidth="1"/>
-    <col min="12" max="12" width="11.6640625" style="4" customWidth="1"/>
-    <col min="13" max="13" width="11.1640625" style="4" bestFit="1" customWidth="1"/>
-    <col min="14" max="17" width="12.33203125" style="4" bestFit="1" customWidth="1"/>
-    <col min="18" max="16384" width="9.1640625" style="1"/>
+    <col min="5" max="7" width="7.1640625" style="4" customWidth="1"/>
+    <col min="8" max="8" width="10.33203125" style="4" bestFit="1" customWidth="1"/>
+    <col min="9" max="12" width="10.83203125" style="4" customWidth="1"/>
+    <col min="13" max="13" width="11.6640625" style="4" customWidth="1"/>
+    <col min="14" max="14" width="11.1640625" style="4" bestFit="1" customWidth="1"/>
+    <col min="15" max="18" width="12.33203125" style="4" bestFit="1" customWidth="1"/>
+    <col min="19" max="16384" width="9.1640625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:19" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A1" s="6" t="s">
         <v>48</v>
       </c>
@@ -1170,46 +1173,49 @@
         <v>47</v>
       </c>
       <c r="E1" s="6" t="s">
+        <v>73</v>
+      </c>
+      <c r="F1" s="6" t="s">
         <v>1</v>
       </c>
-      <c r="F1" s="6" t="s">
+      <c r="G1" s="6" t="s">
         <v>72</v>
       </c>
-      <c r="G1" s="6" t="s">
+      <c r="H1" s="6" t="s">
         <v>67</v>
       </c>
-      <c r="H1" s="6" t="s">
+      <c r="I1" s="6" t="s">
         <v>60</v>
       </c>
-      <c r="I1" s="6" t="s">
+      <c r="J1" s="6" t="s">
         <v>61</v>
       </c>
-      <c r="J1" s="6" t="s">
+      <c r="K1" s="6" t="s">
         <v>62</v>
       </c>
-      <c r="K1" s="6" t="s">
+      <c r="L1" s="6" t="s">
         <v>63</v>
       </c>
-      <c r="L1" s="6" t="s">
+      <c r="M1" s="6" t="s">
         <v>42</v>
       </c>
-      <c r="M1" s="6" t="s">
+      <c r="N1" s="6" t="s">
         <v>43</v>
       </c>
-      <c r="N1" s="6" t="s">
+      <c r="O1" s="6" t="s">
         <v>35</v>
       </c>
-      <c r="O1" s="6" t="s">
+      <c r="P1" s="6" t="s">
         <v>37</v>
       </c>
-      <c r="P1" s="6" t="s">
+      <c r="Q1" s="6" t="s">
         <v>36</v>
       </c>
-      <c r="Q1" s="6" t="s">
+      <c r="R1" s="6" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="2" spans="1:19" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A2" s="6" t="s">
         <v>17</v>
       </c>
@@ -1223,16 +1229,16 @@
         <v>46</v>
       </c>
       <c r="E2" s="3">
+        <v>0.9</v>
+      </c>
+      <c r="F2" s="3">
         <v>0.25</v>
       </c>
-      <c r="F2" s="3">
+      <c r="G2" s="3">
         <v>1</v>
       </c>
-      <c r="G2" s="3">
-        <v>0</v>
-      </c>
       <c r="H2" s="3">
-        <v>0.28999999999999998</v>
+        <v>0</v>
       </c>
       <c r="I2" s="3">
         <v>0.28999999999999998</v>
@@ -1243,27 +1249,30 @@
       <c r="K2" s="3">
         <v>0.28999999999999998</v>
       </c>
-      <c r="L2" s="3" t="s">
+      <c r="L2" s="3">
+        <v>0.28999999999999998</v>
+      </c>
+      <c r="M2" s="3" t="s">
         <v>50</v>
       </c>
-      <c r="M2" s="3" t="s">
+      <c r="N2" s="3" t="s">
         <v>54</v>
       </c>
-      <c r="N2" s="3" t="s">
+      <c r="O2" s="3" t="s">
         <v>55</v>
       </c>
-      <c r="O2" s="3" t="s">
+      <c r="P2" s="3" t="s">
         <v>51</v>
       </c>
-      <c r="P2" s="3" t="s">
+      <c r="Q2" s="3" t="s">
         <v>55</v>
       </c>
-      <c r="Q2" s="3" t="s">
-        <v>49</v>
-      </c>
-      <c r="S2" s="11"/>
-    </row>
-    <row r="3" spans="1:19" x14ac:dyDescent="0.2">
+      <c r="R2" s="3" t="s">
+        <v>49</v>
+      </c>
+      <c r="T2" s="11"/>
+    </row>
+    <row r="3" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A3" s="6" t="s">
         <v>18</v>
       </c>
@@ -1277,16 +1286,16 @@
         <v>46</v>
       </c>
       <c r="E3" s="3">
+        <v>0.9</v>
+      </c>
+      <c r="F3" s="3">
         <v>0.25</v>
       </c>
-      <c r="F3" s="3">
+      <c r="G3" s="3">
         <v>1</v>
       </c>
-      <c r="G3" s="3">
-        <v>0</v>
-      </c>
       <c r="H3" s="3">
-        <v>0.28999999999999998</v>
+        <v>0</v>
       </c>
       <c r="I3" s="3">
         <v>0.28999999999999998</v>
@@ -1297,26 +1306,29 @@
       <c r="K3" s="3">
         <v>0.28999999999999998</v>
       </c>
-      <c r="L3" s="3" t="s">
+      <c r="L3" s="3">
+        <v>0.28999999999999998</v>
+      </c>
+      <c r="M3" s="3" t="s">
         <v>50</v>
       </c>
-      <c r="M3" s="3" t="s">
+      <c r="N3" s="3" t="s">
         <v>54</v>
       </c>
-      <c r="N3" s="3" t="s">
+      <c r="O3" s="3" t="s">
         <v>55</v>
       </c>
-      <c r="O3" s="3" t="s">
+      <c r="P3" s="3" t="s">
         <v>51</v>
       </c>
-      <c r="P3" s="3" t="s">
+      <c r="Q3" s="3" t="s">
         <v>55</v>
       </c>
-      <c r="Q3" s="3" t="s">
-        <v>49</v>
-      </c>
-    </row>
-    <row r="4" spans="1:19" x14ac:dyDescent="0.2">
+      <c r="R3" s="3" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="4" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A4" s="7" t="s">
         <v>19</v>
       </c>
@@ -1330,16 +1342,16 @@
         <v>46</v>
       </c>
       <c r="E4" s="3">
+        <v>0.9</v>
+      </c>
+      <c r="F4" s="3">
         <v>0.84</v>
       </c>
-      <c r="F4" s="3">
+      <c r="G4" s="3">
         <v>1</v>
       </c>
-      <c r="G4" s="3">
-        <v>0</v>
-      </c>
       <c r="H4" s="3">
-        <v>0.35</v>
+        <v>0</v>
       </c>
       <c r="I4" s="3">
         <v>0.35</v>
@@ -1350,26 +1362,29 @@
       <c r="K4" s="3">
         <v>0.35</v>
       </c>
-      <c r="L4" s="3" t="s">
+      <c r="L4" s="3">
+        <v>0.35</v>
+      </c>
+      <c r="M4" s="3" t="s">
         <v>50</v>
       </c>
-      <c r="M4" s="3" t="s">
-        <v>49</v>
-      </c>
       <c r="N4" s="3" t="s">
+        <v>49</v>
+      </c>
+      <c r="O4" s="3" t="s">
         <v>57</v>
-      </c>
-      <c r="O4" s="3" t="s">
-        <v>51</v>
       </c>
       <c r="P4" s="3" t="s">
         <v>51</v>
       </c>
       <c r="Q4" s="3" t="s">
-        <v>49</v>
-      </c>
-    </row>
-    <row r="5" spans="1:19" x14ac:dyDescent="0.2">
+        <v>51</v>
+      </c>
+      <c r="R4" s="3" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="5" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A5" s="7" t="s">
         <v>20</v>
       </c>
@@ -1383,16 +1398,16 @@
         <v>46</v>
       </c>
       <c r="E5" s="3">
+        <v>0.9</v>
+      </c>
+      <c r="F5" s="3">
         <v>0.84</v>
       </c>
-      <c r="F5" s="3">
+      <c r="G5" s="3">
         <v>1</v>
       </c>
-      <c r="G5" s="3">
-        <v>0</v>
-      </c>
       <c r="H5" s="3">
-        <v>0.59</v>
+        <v>0</v>
       </c>
       <c r="I5" s="3">
         <v>0.59</v>
@@ -1403,26 +1418,29 @@
       <c r="K5" s="3">
         <v>0.59</v>
       </c>
-      <c r="L5" s="3" t="s">
+      <c r="L5" s="3">
+        <v>0.59</v>
+      </c>
+      <c r="M5" s="3" t="s">
         <v>50</v>
       </c>
-      <c r="M5" s="3" t="s">
-        <v>49</v>
-      </c>
       <c r="N5" s="3" t="s">
+        <v>49</v>
+      </c>
+      <c r="O5" s="3" t="s">
         <v>57</v>
-      </c>
-      <c r="O5" s="3" t="s">
-        <v>51</v>
       </c>
       <c r="P5" s="3" t="s">
         <v>51</v>
       </c>
       <c r="Q5" s="3" t="s">
-        <v>49</v>
-      </c>
-    </row>
-    <row r="6" spans="1:19" x14ac:dyDescent="0.2">
+        <v>51</v>
+      </c>
+      <c r="R5" s="3" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="6" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A6" s="6" t="s">
         <v>21</v>
       </c>
@@ -1436,16 +1454,16 @@
         <v>46</v>
       </c>
       <c r="E6" s="3">
+        <v>0.9</v>
+      </c>
+      <c r="F6" s="3">
         <v>0.84</v>
       </c>
-      <c r="F6" s="3">
+      <c r="G6" s="3">
         <v>1</v>
       </c>
-      <c r="G6" s="3">
-        <v>0</v>
-      </c>
       <c r="H6" s="3">
-        <v>0.59</v>
+        <v>0</v>
       </c>
       <c r="I6" s="3">
         <v>0.59</v>
@@ -1456,26 +1474,29 @@
       <c r="K6" s="3">
         <v>0.59</v>
       </c>
-      <c r="L6" s="3" t="s">
+      <c r="L6" s="3">
+        <v>0.59</v>
+      </c>
+      <c r="M6" s="3" t="s">
         <v>50</v>
       </c>
-      <c r="M6" s="3" t="s">
-        <v>49</v>
-      </c>
       <c r="N6" s="3" t="s">
+        <v>49</v>
+      </c>
+      <c r="O6" s="3" t="s">
         <v>57</v>
-      </c>
-      <c r="O6" s="3" t="s">
-        <v>51</v>
       </c>
       <c r="P6" s="3" t="s">
         <v>51</v>
       </c>
       <c r="Q6" s="3" t="s">
-        <v>49</v>
-      </c>
-    </row>
-    <row r="7" spans="1:19" x14ac:dyDescent="0.2">
+        <v>51</v>
+      </c>
+      <c r="R6" s="3" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="7" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A7" s="6" t="s">
         <v>31</v>
       </c>
@@ -1489,14 +1510,14 @@
         <v>46</v>
       </c>
       <c r="E7" s="3">
+        <v>0.9</v>
+      </c>
+      <c r="F7" s="3">
         <v>0.84</v>
       </c>
-      <c r="F7" s="3">
+      <c r="G7" s="3">
         <v>1</v>
       </c>
-      <c r="G7" s="3">
-        <v>0</v>
-      </c>
       <c r="H7" s="3">
         <v>0</v>
       </c>
@@ -1509,26 +1530,29 @@
       <c r="K7" s="3">
         <v>0</v>
       </c>
-      <c r="L7" s="3" t="s">
+      <c r="L7" s="3">
+        <v>0</v>
+      </c>
+      <c r="M7" s="3" t="s">
         <v>50</v>
       </c>
-      <c r="M7" s="3" t="s">
-        <v>49</v>
-      </c>
       <c r="N7" s="3" t="s">
+        <v>49</v>
+      </c>
+      <c r="O7" s="3" t="s">
         <v>57</v>
-      </c>
-      <c r="O7" s="3" t="s">
-        <v>51</v>
       </c>
       <c r="P7" s="3" t="s">
         <v>51</v>
       </c>
       <c r="Q7" s="3" t="s">
-        <v>49</v>
-      </c>
-    </row>
-    <row r="8" spans="1:19" x14ac:dyDescent="0.2">
+        <v>51</v>
+      </c>
+      <c r="R7" s="3" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="8" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A8" s="6" t="s">
         <v>22</v>
       </c>
@@ -1542,16 +1566,16 @@
         <v>46</v>
       </c>
       <c r="E8" s="3">
+        <v>0.9</v>
+      </c>
+      <c r="F8" s="3">
         <v>0.84</v>
       </c>
-      <c r="F8" s="3">
+      <c r="G8" s="3">
         <v>1</v>
       </c>
-      <c r="G8" s="3">
-        <v>0</v>
-      </c>
       <c r="H8" s="3">
-        <v>0.59</v>
+        <v>0</v>
       </c>
       <c r="I8" s="3">
         <v>0.59</v>
@@ -1562,26 +1586,29 @@
       <c r="K8" s="3">
         <v>0.59</v>
       </c>
-      <c r="L8" s="3" t="s">
+      <c r="L8" s="3">
+        <v>0.59</v>
+      </c>
+      <c r="M8" s="3" t="s">
         <v>50</v>
       </c>
-      <c r="M8" s="3" t="s">
-        <v>49</v>
-      </c>
       <c r="N8" s="3" t="s">
+        <v>49</v>
+      </c>
+      <c r="O8" s="3" t="s">
         <v>57</v>
-      </c>
-      <c r="O8" s="3" t="s">
-        <v>51</v>
       </c>
       <c r="P8" s="3" t="s">
         <v>51</v>
       </c>
       <c r="Q8" s="3" t="s">
-        <v>49</v>
-      </c>
-    </row>
-    <row r="9" spans="1:19" x14ac:dyDescent="0.2">
+        <v>51</v>
+      </c>
+      <c r="R8" s="3" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="9" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A9" s="6" t="s">
         <v>23</v>
       </c>
@@ -1595,16 +1622,16 @@
         <v>46</v>
       </c>
       <c r="E9" s="3">
+        <v>0.9</v>
+      </c>
+      <c r="F9" s="3">
         <v>0.7</v>
       </c>
-      <c r="F9" s="3">
+      <c r="G9" s="3">
         <v>1</v>
       </c>
-      <c r="G9" s="3">
-        <v>0</v>
-      </c>
       <c r="H9" s="3">
-        <v>0.1</v>
+        <v>0</v>
       </c>
       <c r="I9" s="3">
         <v>0.1</v>
@@ -1615,26 +1642,29 @@
       <c r="K9" s="3">
         <v>0.1</v>
       </c>
-      <c r="L9" s="3" t="s">
+      <c r="L9" s="3">
+        <v>0.1</v>
+      </c>
+      <c r="M9" s="3" t="s">
         <v>50</v>
       </c>
-      <c r="M9" s="3" t="s">
-        <v>49</v>
-      </c>
       <c r="N9" s="3" t="s">
+        <v>49</v>
+      </c>
+      <c r="O9" s="3" t="s">
         <v>57</v>
-      </c>
-      <c r="O9" s="3" t="s">
-        <v>51</v>
       </c>
       <c r="P9" s="3" t="s">
         <v>51</v>
       </c>
       <c r="Q9" s="3" t="s">
-        <v>49</v>
-      </c>
-    </row>
-    <row r="10" spans="1:19" x14ac:dyDescent="0.2">
+        <v>51</v>
+      </c>
+      <c r="R9" s="3" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="10" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A10" s="6" t="s">
         <v>66</v>
       </c>
@@ -1648,16 +1678,16 @@
         <v>46</v>
       </c>
       <c r="E10" s="3">
+        <v>0.9</v>
+      </c>
+      <c r="F10" s="3">
         <v>0.67</v>
       </c>
-      <c r="F10" s="3">
+      <c r="G10" s="3">
         <v>1</v>
       </c>
-      <c r="G10" s="3">
-        <v>0</v>
-      </c>
       <c r="H10" s="3">
-        <v>0.35</v>
+        <v>0</v>
       </c>
       <c r="I10" s="3">
         <v>0.35</v>
@@ -1668,26 +1698,29 @@
       <c r="K10" s="3">
         <v>0.35</v>
       </c>
-      <c r="L10" s="3" t="s">
+      <c r="L10" s="3">
+        <v>0.35</v>
+      </c>
+      <c r="M10" s="3" t="s">
         <v>50</v>
       </c>
-      <c r="M10" s="3" t="s">
-        <v>49</v>
-      </c>
       <c r="N10" s="3" t="s">
+        <v>49</v>
+      </c>
+      <c r="O10" s="3" t="s">
         <v>57</v>
-      </c>
-      <c r="O10" s="3" t="s">
-        <v>51</v>
       </c>
       <c r="P10" s="3" t="s">
         <v>51</v>
       </c>
       <c r="Q10" s="3" t="s">
-        <v>49</v>
-      </c>
-    </row>
-    <row r="11" spans="1:19" x14ac:dyDescent="0.2">
+        <v>51</v>
+      </c>
+      <c r="R10" s="3" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="11" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A11" s="6" t="s">
         <v>24</v>
       </c>
@@ -1701,16 +1734,16 @@
         <v>46</v>
       </c>
       <c r="E11" s="3">
+        <v>0.9</v>
+      </c>
+      <c r="F11" s="3">
         <v>0.67</v>
       </c>
-      <c r="F11" s="3">
+      <c r="G11" s="3">
         <v>1</v>
       </c>
-      <c r="G11" s="3">
-        <v>0</v>
-      </c>
       <c r="H11" s="3">
-        <v>0.35</v>
+        <v>0</v>
       </c>
       <c r="I11" s="3">
         <v>0.35</v>
@@ -1721,26 +1754,29 @@
       <c r="K11" s="3">
         <v>0.35</v>
       </c>
-      <c r="L11" s="3" t="s">
+      <c r="L11" s="3">
+        <v>0.35</v>
+      </c>
+      <c r="M11" s="3" t="s">
         <v>50</v>
       </c>
-      <c r="M11" s="3" t="s">
-        <v>49</v>
-      </c>
       <c r="N11" s="3" t="s">
+        <v>49</v>
+      </c>
+      <c r="O11" s="3" t="s">
         <v>56</v>
-      </c>
-      <c r="O11" s="3" t="s">
-        <v>51</v>
       </c>
       <c r="P11" s="3" t="s">
         <v>51</v>
       </c>
       <c r="Q11" s="3" t="s">
-        <v>49</v>
-      </c>
-    </row>
-    <row r="12" spans="1:19" x14ac:dyDescent="0.2">
+        <v>51</v>
+      </c>
+      <c r="R11" s="3" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="12" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A12" s="6" t="s">
         <v>25</v>
       </c>
@@ -1754,16 +1790,16 @@
         <v>46</v>
       </c>
       <c r="E12" s="3">
+        <v>0.9</v>
+      </c>
+      <c r="F12" s="3">
         <v>0.84</v>
       </c>
-      <c r="F12" s="3">
+      <c r="G12" s="3">
         <v>1</v>
       </c>
-      <c r="G12" s="3">
-        <v>0</v>
-      </c>
       <c r="H12" s="3">
-        <v>0.35</v>
+        <v>0</v>
       </c>
       <c r="I12" s="3">
         <v>0.35</v>
@@ -1774,26 +1810,29 @@
       <c r="K12" s="3">
         <v>0.35</v>
       </c>
-      <c r="L12" s="3" t="s">
+      <c r="L12" s="3">
+        <v>0.35</v>
+      </c>
+      <c r="M12" s="3" t="s">
         <v>50</v>
       </c>
-      <c r="M12" s="3" t="s">
-        <v>49</v>
-      </c>
       <c r="N12" s="3" t="s">
+        <v>49</v>
+      </c>
+      <c r="O12" s="3" t="s">
         <v>57</v>
-      </c>
-      <c r="O12" s="3" t="s">
-        <v>51</v>
       </c>
       <c r="P12" s="3" t="s">
         <v>51</v>
       </c>
       <c r="Q12" s="3" t="s">
-        <v>49</v>
-      </c>
-    </row>
-    <row r="13" spans="1:19" x14ac:dyDescent="0.2">
+        <v>51</v>
+      </c>
+      <c r="R12" s="3" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="13" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A13" s="6" t="s">
         <v>26</v>
       </c>
@@ -1807,16 +1846,16 @@
         <v>46</v>
       </c>
       <c r="E13" s="3">
+        <v>0.9</v>
+      </c>
+      <c r="F13" s="3">
         <v>0.67</v>
       </c>
-      <c r="F13" s="3">
+      <c r="G13" s="3">
         <v>1</v>
       </c>
-      <c r="G13" s="3">
-        <v>0</v>
-      </c>
       <c r="H13" s="3">
-        <v>0.35</v>
+        <v>0</v>
       </c>
       <c r="I13" s="3">
         <v>0.35</v>
@@ -1827,26 +1866,29 @@
       <c r="K13" s="3">
         <v>0.35</v>
       </c>
-      <c r="L13" s="3" t="s">
+      <c r="L13" s="3">
+        <v>0.35</v>
+      </c>
+      <c r="M13" s="3" t="s">
         <v>50</v>
       </c>
-      <c r="M13" s="3" t="s">
-        <v>49</v>
-      </c>
       <c r="N13" s="3" t="s">
+        <v>49</v>
+      </c>
+      <c r="O13" s="3" t="s">
         <v>56</v>
-      </c>
-      <c r="O13" s="3" t="s">
-        <v>51</v>
       </c>
       <c r="P13" s="3" t="s">
         <v>51</v>
       </c>
       <c r="Q13" s="3" t="s">
-        <v>49</v>
-      </c>
-    </row>
-    <row r="14" spans="1:19" x14ac:dyDescent="0.2">
+        <v>51</v>
+      </c>
+      <c r="R13" s="3" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="14" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A14" s="6" t="s">
         <v>27</v>
       </c>
@@ -1860,16 +1902,16 @@
         <v>46</v>
       </c>
       <c r="E14" s="3">
-        <v>0</v>
+        <v>0.9</v>
       </c>
       <c r="F14" s="3">
+        <v>0</v>
+      </c>
+      <c r="G14" s="3">
         <v>1</v>
       </c>
-      <c r="G14" s="3">
-        <v>0</v>
-      </c>
       <c r="H14" s="3">
-        <v>0.35</v>
+        <v>0</v>
       </c>
       <c r="I14" s="3">
         <v>0.35</v>
@@ -1880,26 +1922,29 @@
       <c r="K14" s="3">
         <v>0.35</v>
       </c>
-      <c r="L14" s="3" t="s">
+      <c r="L14" s="3">
+        <v>0.35</v>
+      </c>
+      <c r="M14" s="3" t="s">
         <v>50</v>
       </c>
-      <c r="M14" s="3" t="s">
-        <v>49</v>
-      </c>
       <c r="N14" s="3" t="s">
+        <v>49</v>
+      </c>
+      <c r="O14" s="3" t="s">
         <v>57</v>
       </c>
-      <c r="O14" s="3" t="s">
+      <c r="P14" s="3" t="s">
         <v>51</v>
       </c>
-      <c r="P14" s="3" t="s">
+      <c r="Q14" s="3" t="s">
         <v>55</v>
       </c>
-      <c r="Q14" s="3" t="s">
-        <v>53</v>
-      </c>
-    </row>
-    <row r="15" spans="1:19" x14ac:dyDescent="0.2">
+      <c r="R14" s="3" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="15" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A15" s="6" t="s">
         <v>28</v>
       </c>
@@ -1913,13 +1958,13 @@
         <v>46</v>
       </c>
       <c r="E15" s="3">
-        <v>1</v>
+        <v>0.9</v>
       </c>
       <c r="F15" s="3">
         <v>1</v>
       </c>
       <c r="G15" s="3">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H15" s="3">
         <v>0</v>
@@ -1933,26 +1978,29 @@
       <c r="K15" s="3">
         <v>0</v>
       </c>
-      <c r="L15" s="3" t="s">
+      <c r="L15" s="3">
+        <v>0</v>
+      </c>
+      <c r="M15" s="3" t="s">
         <v>50</v>
       </c>
-      <c r="M15" s="3" t="s">
-        <v>49</v>
-      </c>
       <c r="N15" s="3" t="s">
+        <v>49</v>
+      </c>
+      <c r="O15" s="3" t="s">
         <v>57</v>
-      </c>
-      <c r="O15" s="3" t="s">
-        <v>51</v>
       </c>
       <c r="P15" s="3" t="s">
         <v>51</v>
       </c>
       <c r="Q15" s="3" t="s">
-        <v>49</v>
-      </c>
-    </row>
-    <row r="16" spans="1:19" x14ac:dyDescent="0.2">
+        <v>51</v>
+      </c>
+      <c r="R15" s="3" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="16" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A16" s="6" t="s">
         <v>29</v>
       </c>
@@ -1966,16 +2014,16 @@
         <v>46</v>
       </c>
       <c r="E16" s="3">
-        <v>0</v>
+        <v>0.9</v>
       </c>
       <c r="F16" s="3">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G16" s="3">
         <v>1</v>
       </c>
       <c r="H16" s="3">
-        <v>0.5</v>
+        <v>1</v>
       </c>
       <c r="I16" s="3">
         <v>0.5</v>
@@ -1986,26 +2034,29 @@
       <c r="K16" s="3">
         <v>0.5</v>
       </c>
-      <c r="L16" s="3" t="s">
+      <c r="L16" s="3">
+        <v>0.5</v>
+      </c>
+      <c r="M16" s="3" t="s">
         <v>50</v>
       </c>
-      <c r="M16" s="3" t="s">
+      <c r="N16" s="3" t="s">
         <v>52</v>
       </c>
-      <c r="N16" s="3" t="s">
-        <v>49</v>
-      </c>
       <c r="O16" s="3" t="s">
+        <v>49</v>
+      </c>
+      <c r="P16" s="3" t="s">
         <v>51</v>
       </c>
-      <c r="P16" s="3" t="s">
+      <c r="Q16" s="3" t="s">
         <v>55</v>
       </c>
-      <c r="Q16" s="3" t="s">
-        <v>53</v>
-      </c>
-    </row>
-    <row r="17" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="R16" s="3" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="17" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A17" s="6" t="s">
         <v>30</v>
       </c>
@@ -2019,13 +2070,13 @@
         <v>46</v>
       </c>
       <c r="E17" s="3">
-        <v>1</v>
+        <v>0.9</v>
       </c>
       <c r="F17" s="3">
         <v>1</v>
       </c>
       <c r="G17" s="3">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H17" s="3">
         <v>0</v>
@@ -2039,26 +2090,29 @@
       <c r="K17" s="3">
         <v>0</v>
       </c>
-      <c r="L17" s="3" t="s">
+      <c r="L17" s="3">
+        <v>0</v>
+      </c>
+      <c r="M17" s="3" t="s">
         <v>50</v>
       </c>
-      <c r="M17" s="3" t="s">
-        <v>49</v>
-      </c>
       <c r="N17" s="3" t="s">
         <v>49</v>
       </c>
       <c r="O17" s="3" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="P17" s="3" t="s">
         <v>51</v>
       </c>
       <c r="Q17" s="3" t="s">
-        <v>49</v>
-      </c>
-    </row>
-    <row r="18" spans="1:17" x14ac:dyDescent="0.2">
+        <v>51</v>
+      </c>
+      <c r="R17" s="3" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="18" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A18" s="6" t="s">
         <v>39</v>
       </c>
@@ -2072,16 +2126,16 @@
         <v>46</v>
       </c>
       <c r="E18" s="3">
+        <v>0.9</v>
+      </c>
+      <c r="F18" s="3">
         <v>0.67</v>
       </c>
-      <c r="F18" s="3">
+      <c r="G18" s="3">
         <v>1</v>
       </c>
-      <c r="G18" s="3">
-        <v>0</v>
-      </c>
       <c r="H18" s="3">
-        <v>0.35</v>
+        <v>0</v>
       </c>
       <c r="I18" s="3">
         <v>0.35</v>
@@ -2092,26 +2146,29 @@
       <c r="K18" s="3">
         <v>0.35</v>
       </c>
-      <c r="L18" s="3" t="s">
+      <c r="L18" s="3">
+        <v>0.35</v>
+      </c>
+      <c r="M18" s="3" t="s">
         <v>50</v>
       </c>
-      <c r="M18" s="3" t="s">
-        <v>49</v>
-      </c>
       <c r="N18" s="3" t="s">
+        <v>49</v>
+      </c>
+      <c r="O18" s="3" t="s">
         <v>56</v>
-      </c>
-      <c r="O18" s="3" t="s">
-        <v>51</v>
       </c>
       <c r="P18" s="3" t="s">
         <v>51</v>
       </c>
       <c r="Q18" s="3" t="s">
-        <v>49</v>
-      </c>
-    </row>
-    <row r="19" spans="1:17" x14ac:dyDescent="0.2">
+        <v>51</v>
+      </c>
+      <c r="R18" s="3" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="19" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A19" s="6" t="s">
         <v>40</v>
       </c>
@@ -2125,16 +2182,16 @@
         <v>46</v>
       </c>
       <c r="E19" s="3">
+        <v>0.9</v>
+      </c>
+      <c r="F19" s="3">
         <v>0.67</v>
       </c>
-      <c r="F19" s="3">
+      <c r="G19" s="3">
         <v>1</v>
       </c>
-      <c r="G19" s="3">
-        <v>0</v>
-      </c>
       <c r="H19" s="3">
-        <v>0.35</v>
+        <v>0</v>
       </c>
       <c r="I19" s="3">
         <v>0.35</v>
@@ -2145,26 +2202,29 @@
       <c r="K19" s="3">
         <v>0.35</v>
       </c>
-      <c r="L19" s="3" t="s">
+      <c r="L19" s="3">
+        <v>0.35</v>
+      </c>
+      <c r="M19" s="3" t="s">
         <v>50</v>
       </c>
-      <c r="M19" s="3" t="s">
-        <v>49</v>
-      </c>
       <c r="N19" s="3" t="s">
+        <v>49</v>
+      </c>
+      <c r="O19" s="3" t="s">
         <v>56</v>
-      </c>
-      <c r="O19" s="3" t="s">
-        <v>51</v>
       </c>
       <c r="P19" s="3" t="s">
         <v>51</v>
       </c>
       <c r="Q19" s="3" t="s">
-        <v>49</v>
-      </c>
-    </row>
-    <row r="20" spans="1:17" x14ac:dyDescent="0.2">
+        <v>51</v>
+      </c>
+      <c r="R19" s="3" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="20" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A20" s="6" t="s">
         <v>41</v>
       </c>
@@ -2178,16 +2238,16 @@
         <v>46</v>
       </c>
       <c r="E20" s="3">
+        <v>0.9</v>
+      </c>
+      <c r="F20" s="3">
         <v>0.67</v>
       </c>
-      <c r="F20" s="3">
+      <c r="G20" s="3">
         <v>1</v>
       </c>
-      <c r="G20" s="3">
-        <v>0</v>
-      </c>
       <c r="H20" s="3">
-        <v>0.35</v>
+        <v>0</v>
       </c>
       <c r="I20" s="3">
         <v>0.35</v>
@@ -2198,22 +2258,25 @@
       <c r="K20" s="3">
         <v>0.35</v>
       </c>
-      <c r="L20" s="3" t="s">
+      <c r="L20" s="3">
+        <v>0.35</v>
+      </c>
+      <c r="M20" s="3" t="s">
         <v>50</v>
       </c>
-      <c r="M20" s="3" t="s">
-        <v>49</v>
-      </c>
       <c r="N20" s="3" t="s">
+        <v>49</v>
+      </c>
+      <c r="O20" s="3" t="s">
         <v>56</v>
-      </c>
-      <c r="O20" s="3" t="s">
-        <v>51</v>
       </c>
       <c r="P20" s="3" t="s">
         <v>51</v>
       </c>
       <c r="Q20" s="3" t="s">
+        <v>51</v>
+      </c>
+      <c r="R20" s="3" t="s">
         <v>49</v>
       </c>
     </row>

</xml_diff>